<commit_message>
Update backlog, setup evironment
</commit_message>
<xml_diff>
--- a/QA Backlog.xlsx
+++ b/QA Backlog.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="94">
   <si>
     <t>No</t>
   </si>
@@ -286,6 +286,18 @@
   </si>
   <si>
     <t>New answers or replies will show at real time without refreshing page</t>
+  </si>
+  <si>
+    <t>Design get forget password page</t>
+  </si>
+  <si>
+    <t>Pop-up form</t>
+  </si>
+  <si>
+    <t>Create guest use-cases</t>
+  </si>
+  <si>
+    <t>Start after KhangTN commits overall usecase</t>
   </si>
 </sst>
 </file>
@@ -386,13 +398,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -404,9 +422,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -742,7 +757,7 @@
       <c r="A2" s="2">
         <v>1</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="8" t="s">
         <v>10</v>
       </c>
       <c r="C2" s="2" t="s">
@@ -756,7 +771,7 @@
       <c r="A3" s="2">
         <v>2</v>
       </c>
-      <c r="B3" s="6"/>
+      <c r="B3" s="8"/>
       <c r="C3" s="2" t="s">
         <v>4</v>
       </c>
@@ -768,7 +783,7 @@
       <c r="A4" s="2">
         <v>3</v>
       </c>
-      <c r="B4" s="6"/>
+      <c r="B4" s="8"/>
       <c r="C4" s="2" t="s">
         <v>8</v>
       </c>
@@ -804,7 +819,7 @@
       <c r="A7" s="2">
         <v>6</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="9" t="s">
         <v>12</v>
       </c>
       <c r="C7" s="2" t="s">
@@ -818,7 +833,7 @@
       <c r="A8" s="2">
         <v>7</v>
       </c>
-      <c r="B8" s="7"/>
+      <c r="B8" s="9"/>
       <c r="C8" s="2" t="s">
         <v>14</v>
       </c>
@@ -830,7 +845,7 @@
       <c r="A9" s="2">
         <v>8</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="B9" s="9" t="s">
         <v>16</v>
       </c>
       <c r="C9" s="2" t="s">
@@ -844,7 +859,7 @@
       <c r="A10" s="2">
         <v>9</v>
       </c>
-      <c r="B10" s="7"/>
+      <c r="B10" s="9"/>
       <c r="C10" s="2" t="s">
         <v>19</v>
       </c>
@@ -856,7 +871,7 @@
       <c r="A11" s="2">
         <v>10</v>
       </c>
-      <c r="B11" s="7" t="s">
+      <c r="B11" s="9" t="s">
         <v>38</v>
       </c>
       <c r="C11" s="2" t="s">
@@ -870,7 +885,7 @@
       <c r="A12" s="2">
         <v>11</v>
       </c>
-      <c r="B12" s="7"/>
+      <c r="B12" s="9"/>
       <c r="C12" s="2" t="s">
         <v>41</v>
       </c>
@@ -1002,7 +1017,7 @@
       <c r="A23" s="2">
         <v>22</v>
       </c>
-      <c r="B23" s="8" t="s">
+      <c r="B23" s="10" t="s">
         <v>48</v>
       </c>
       <c r="C23" s="2" t="s">
@@ -1016,7 +1031,7 @@
       <c r="A24" s="2">
         <v>23</v>
       </c>
-      <c r="B24" s="9"/>
+      <c r="B24" s="11"/>
       <c r="C24" s="2" t="s">
         <v>50</v>
       </c>
@@ -1041,8 +1056,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1139,7 +1154,7 @@
         <v>80</v>
       </c>
       <c r="E5" s="2">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>86</v>
@@ -1159,12 +1174,14 @@
       <c r="B6" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="C6" s="2"/>
+      <c r="C6" s="2" t="s">
+        <v>91</v>
+      </c>
       <c r="D6" s="2" t="s">
         <v>80</v>
       </c>
       <c r="E6" s="2">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>86</v>
@@ -1182,14 +1199,14 @@
         <v>4</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>68</v>
+        <v>90</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="2" t="s">
         <v>80</v>
       </c>
       <c r="E7" s="2">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>86</v>
@@ -1207,14 +1224,14 @@
         <v>5</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C8" s="2"/>
       <c r="D8" s="2" t="s">
         <v>81</v>
       </c>
       <c r="E8" s="2">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F8" s="2" t="s">
         <v>86</v>
@@ -1232,14 +1249,14 @@
         <v>6</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="2" t="s">
         <v>81</v>
       </c>
       <c r="E9" s="2">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F9" s="2" t="s">
         <v>86</v>
@@ -1253,18 +1270,18 @@
       <c r="M9" s="2"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A10" s="10">
+      <c r="A10" s="2">
         <v>7</v>
       </c>
-      <c r="B10" s="7" t="s">
-        <v>71</v>
+      <c r="B10" s="2" t="s">
+        <v>70</v>
       </c>
       <c r="C10" s="2"/>
       <c r="D10" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="E10" s="2">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="F10" s="2" t="s">
         <v>86</v>
@@ -1278,14 +1295,18 @@
       <c r="M10" s="2"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A11" s="10"/>
-      <c r="B11" s="7"/>
+      <c r="A11" s="2">
+        <v>8</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>71</v>
+      </c>
       <c r="C11" s="2"/>
       <c r="D11" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E11" s="2">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F11" s="2" t="s">
         <v>86</v>
@@ -1300,7 +1321,7 @@
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>72</v>
@@ -1325,7 +1346,7 @@
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>73</v>
@@ -1350,7 +1371,7 @@
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>74</v>
@@ -1375,14 +1396,16 @@
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="C15" s="2"/>
+        <v>92</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>93</v>
+      </c>
       <c r="D15" s="2" t="s">
-        <v>58</v>
+        <v>80</v>
       </c>
       <c r="E15" s="2">
         <v>10</v>
@@ -1403,14 +1426,14 @@
         <v>12</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C16" s="2"/>
       <c r="D16" s="2" t="s">
-        <v>79</v>
+        <v>58</v>
       </c>
       <c r="E16" s="2">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F16" s="2" t="s">
         <v>86</v>
@@ -1424,18 +1447,18 @@
       <c r="M16" s="2"/>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A17" s="10">
+      <c r="A17" s="2">
         <v>13</v>
       </c>
-      <c r="B17" s="7" t="s">
-        <v>77</v>
+      <c r="B17" s="2" t="s">
+        <v>76</v>
       </c>
       <c r="C17" s="2"/>
       <c r="D17" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E17" s="2">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="F17" s="2" t="s">
         <v>86</v>
@@ -1449,8 +1472,12 @@
       <c r="M17" s="2"/>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A18" s="10"/>
-      <c r="B18" s="7"/>
+      <c r="A18" s="2">
+        <v>14</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>77</v>
+      </c>
       <c r="C18" s="2"/>
       <c r="D18" s="2" t="s">
         <v>81</v>
@@ -1471,7 +1498,7 @@
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>78</v>
@@ -1513,7 +1540,7 @@
       </c>
       <c r="C24" s="2">
         <f>SUMIF(D4:D19,B24,E4:E19)</f>
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.2">
@@ -1531,7 +1558,7 @@
       </c>
       <c r="C26" s="2">
         <f>SUMIF(D4:D19,B26,E4:E19)</f>
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.2">
@@ -1540,7 +1567,7 @@
       </c>
       <c r="C27" s="2">
         <f>SUMIF(D4:D19,B27,E4:E19)</f>
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.2">
@@ -1581,12 +1608,6 @@
       <c r="C34" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="A17:A18"/>
-    <mergeCell ref="B17:B18"/>
-  </mergeCells>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D4:D19">
       <formula1>"MinhKH, KhangTN, ThiTD, TungTD"</formula1>

</xml_diff>

<commit_message>
update backlog for MinhKH and ThiTD
</commit_message>
<xml_diff>
--- a/QA Backlog.xlsx
+++ b/QA Backlog.xlsx
@@ -300,10 +300,10 @@
     <t>Start after KhangTN commits overall usecase</t>
   </si>
   <si>
-    <t>Waiting for Approval</t>
-  </si>
-  <si>
     <t>In process</t>
+  </si>
+  <si>
+    <t>Completed</t>
   </si>
 </sst>
 </file>
@@ -1063,7 +1063,7 @@
   <dimension ref="A1:M34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1138,7 +1138,7 @@
         <v>10</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
@@ -1315,7 +1315,7 @@
         <v>4</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
@@ -1442,7 +1442,7 @@
         <v>12</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>

</xml_diff>

<commit_message>
update minhkh and khanhtn backlog
</commit_message>
<xml_diff>
--- a/QA Backlog.xlsx
+++ b/QA Backlog.xlsx
@@ -1063,7 +1063,7 @@
   <dimension ref="A1:M34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1390,7 +1390,7 @@
         <v>15</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>86</v>
+        <v>95</v>
       </c>
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
@@ -1442,7 +1442,7 @@
         <v>12</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>

</xml_diff>

<commit_message>
Approve setup environment for Khang
</commit_message>
<xml_diff>
--- a/QA Backlog.xlsx
+++ b/QA Backlog.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\study\Capstone\Document\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="240" yWindow="60" windowWidth="20115" windowHeight="8010" activeTab="1"/>
   </bookViews>
@@ -16,7 +11,7 @@
     <sheet name="Sprint 1" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="152511" concurrentCalc="0"/>
+  <calcPr calcId="144525" concurrentCalc="0"/>
 </workbook>
 </file>
 
@@ -497,7 +492,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -532,7 +527,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1074,7 +1069,7 @@
   <dimension ref="A1:M34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1376,7 +1371,7 @@
         <v>8</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>

</xml_diff>

<commit_message>
Update backlog, Upload report full version
</commit_message>
<xml_diff>
--- a/QA Backlog.xlsx
+++ b/QA Backlog.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="60" windowWidth="20115" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="60" windowWidth="20115" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="91">
   <si>
     <t>No</t>
   </si>
@@ -24,9 +24,6 @@
     <t>Function</t>
   </si>
   <si>
-    <t>Detail</t>
-  </si>
-  <si>
     <t>Description</t>
   </si>
   <si>
@@ -45,18 +42,9 @@
     <t>Get forgotton password</t>
   </si>
   <si>
-    <t>Reseting password if forgetting</t>
-  </si>
-  <si>
-    <t>Autheticate</t>
-  </si>
-  <si>
     <t>Create class</t>
   </si>
   <si>
-    <t>Create post</t>
-  </si>
-  <si>
     <t>Create article, question, answer</t>
   </si>
   <si>
@@ -66,9 +54,6 @@
     <t>User post an article, ask a question or answer a question</t>
   </si>
   <si>
-    <t>Invite user</t>
-  </si>
-  <si>
     <t>Invite teacher</t>
   </si>
   <si>
@@ -132,9 +117,6 @@
     <t>Search</t>
   </si>
   <si>
-    <t>Accept/Deny</t>
-  </si>
-  <si>
     <t>Accept/Deny an invitation</t>
   </si>
   <si>
@@ -162,9 +144,6 @@
     <t>Teachers manage students in their class</t>
   </si>
   <si>
-    <t>Manage website</t>
-  </si>
-  <si>
     <t>Manage users</t>
   </si>
   <si>
@@ -307,6 +286,9 @@
   </si>
   <si>
     <t>Waiting for Approval</t>
+  </si>
+  <si>
+    <t>Resetting password if forgetting</t>
   </si>
 </sst>
 </file>
@@ -354,7 +336,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -390,24 +372,11 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -418,18 +387,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -736,22 +693,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D24"/>
+  <dimension ref="A1:C24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="1"/>
     <col min="2" max="2" width="28.42578125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="32.7109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="100.85546875" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="1"/>
+    <col min="3" max="3" width="100.85546875" style="1" customWidth="1"/>
+    <col min="4" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="18" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -761,304 +717,261 @@
       <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>1</v>
       </c>
-      <c r="B2" s="8" t="s">
-        <v>10</v>
+      <c r="B2" s="2" t="s">
+        <v>4</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>2</v>
       </c>
-      <c r="B3" s="8"/>
+      <c r="B3" s="2" t="s">
+        <v>3</v>
+      </c>
       <c r="C3" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>3</v>
       </c>
-      <c r="B4" s="8"/>
+      <c r="B4" s="2" t="s">
+        <v>7</v>
+      </c>
       <c r="C4" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+        <v>29</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+        <v>8</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>6</v>
       </c>
-      <c r="B7" s="9" t="s">
-        <v>12</v>
+      <c r="B7" s="2" t="s">
+        <v>9</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>7</v>
       </c>
-      <c r="B8" s="9"/>
+      <c r="B8" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="C8" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>8</v>
       </c>
-      <c r="B9" s="9" t="s">
-        <v>16</v>
+      <c r="B9" s="2" t="s">
+        <v>12</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>9</v>
       </c>
-      <c r="B10" s="9"/>
+      <c r="B10" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="C10" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>10</v>
       </c>
-      <c r="B11" s="9" t="s">
-        <v>38</v>
+      <c r="B11" s="2" t="s">
+        <v>33</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <v>11</v>
       </c>
-      <c r="B12" s="9"/>
+      <c r="B12" s="2" t="s">
+        <v>35</v>
+      </c>
       <c r="C12" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
         <v>12</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+        <v>17</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
         <v>13</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+        <v>39</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
         <v>14</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+        <v>38</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
         <v>15</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
         <v>16</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+        <v>19</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
         <v>17</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+        <v>20</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
         <v>18</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+        <v>23</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
         <v>19</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+        <v>25</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="2">
         <v>20</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+        <v>27</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="2">
         <v>21</v>
       </c>
       <c r="B22" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C22" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C22" s="2"/>
-      <c r="D22" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="2">
         <v>22</v>
       </c>
-      <c r="B23" s="10" t="s">
-        <v>48</v>
+      <c r="B23" s="2" t="s">
+        <v>42</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="2">
         <v>23</v>
       </c>
-      <c r="B24" s="11"/>
+      <c r="B24" s="2" t="s">
+        <v>43</v>
+      </c>
       <c r="C24" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="5">
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="B23:B24"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -1068,7 +981,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
@@ -1085,7 +998,7 @@
   <sheetData>
     <row r="1" spans="1:13" ht="25.5" x14ac:dyDescent="0.35">
       <c r="B1" s="4" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
@@ -1093,40 +1006,40 @@
         <v>0</v>
       </c>
       <c r="B3" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="H3" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="I3" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="D3" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="E3" s="5" t="s">
+      <c r="J3" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="K3" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="G3" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="H3" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="I3" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="J3" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="K3" s="5" t="s">
-        <v>63</v>
-      </c>
       <c r="L3" s="5" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="M3" s="5" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
@@ -1134,17 +1047,17 @@
         <v>1</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="2" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="E4" s="2">
         <v>10</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
@@ -1159,17 +1072,17 @@
         <v>2</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="C5" s="2"/>
       <c r="D5" s="2" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="E5" s="2">
         <v>6</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
@@ -1184,19 +1097,19 @@
         <v>3</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="E6" s="2">
         <v>6</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
@@ -1211,17 +1124,17 @@
         <v>4</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="2" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="E7" s="2">
         <v>6</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
@@ -1236,17 +1149,17 @@
         <v>5</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="C8" s="2"/>
       <c r="D8" s="2" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="E8" s="2">
         <v>8</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
@@ -1261,17 +1174,17 @@
         <v>6</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="2" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="E9" s="2">
         <v>8</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
@@ -1286,17 +1199,17 @@
         <v>7</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="C10" s="2"/>
       <c r="D10" s="2" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="E10" s="2">
         <v>8</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
@@ -1311,17 +1224,17 @@
         <v>8</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="C11" s="2"/>
       <c r="D11" s="2" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="E11" s="2">
         <v>4</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
@@ -1336,17 +1249,17 @@
         <v>9</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="C12" s="2"/>
       <c r="D12" s="2" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="E12" s="2">
         <v>3</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
@@ -1361,17 +1274,17 @@
         <v>10</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" s="2" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="E13" s="2">
         <v>8</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
@@ -1386,17 +1299,17 @@
         <v>11</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="C14" s="2"/>
       <c r="D14" s="2" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="E14" s="2">
         <v>15</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
@@ -1411,19 +1324,19 @@
         <v>12</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="E15" s="2">
         <v>10</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
@@ -1438,17 +1351,17 @@
         <v>12</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="C16" s="2"/>
       <c r="D16" s="2" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="E16" s="2">
         <v>12</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
@@ -1463,17 +1376,17 @@
         <v>13</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="C17" s="2"/>
       <c r="D17" s="2" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="E17" s="2">
         <v>10</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
@@ -1488,17 +1401,17 @@
         <v>14</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="C18" s="2"/>
       <c r="D18" s="2" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="E18" s="2">
         <v>8</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
@@ -1513,17 +1426,17 @@
         <v>15</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="C19" s="2"/>
       <c r="D19" s="2" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="E19" s="2">
         <v>3</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
@@ -1535,20 +1448,20 @@
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B22" s="1" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B23" s="5" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B24" s="2" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="C24" s="2">
         <f>SUMIF(D4:D19,B24,E4:E19)</f>
@@ -1557,7 +1470,7 @@
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B25" s="2" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="C25" s="2">
         <f>SUMIF(D4:D19,B25,E4:E19)</f>
@@ -1566,7 +1479,7 @@
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B26" s="2" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="C26" s="2">
         <f>SUMIF(D4:D19,B26,E4:E19)</f>
@@ -1575,7 +1488,7 @@
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B27" s="2" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="C27" s="2">
         <f>SUMIF(D4:D19,B27,E4:E19)</f>
@@ -1584,38 +1497,38 @@
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B29" s="1" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B30" s="5" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B31" s="2" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="C31" s="2"/>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B32" s="2" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="C32" s="2"/>
     </row>
     <row r="33" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B33" s="2" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="C33" s="2"/>
     </row>
     <row r="34" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B34" s="2" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="C34" s="2"/>
     </row>

</xml_diff>

<commit_message>
Update backlog status sprint 1, create sprint 2
</commit_message>
<xml_diff>
--- a/QA Backlog.xlsx
+++ b/QA Backlog.xlsx
@@ -1,27 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\study\Capstone\Document\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="60" windowWidth="20115" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="60" windowWidth="20115" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="1" r:id="rId1"/>
     <sheet name="Sprint 1" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sprint 2" sheetId="4" r:id="rId3"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="152511" concurrentCalc="0"/>
+  <calcPr calcId="144525" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="118">
   <si>
     <t>No</t>
   </si>
@@ -29,9 +25,6 @@
     <t>Function</t>
   </si>
   <si>
-    <t>Detail</t>
-  </si>
-  <si>
     <t>Description</t>
   </si>
   <si>
@@ -53,15 +46,9 @@
     <t>Reseting password if forgetting</t>
   </si>
   <si>
-    <t>Autheticate</t>
-  </si>
-  <si>
     <t>Create class</t>
   </si>
   <si>
-    <t>Create post</t>
-  </si>
-  <si>
     <t>Create article, question, answer</t>
   </si>
   <si>
@@ -71,9 +58,6 @@
     <t>User post an article, ask a question or answer a question</t>
   </si>
   <si>
-    <t>Invite user</t>
-  </si>
-  <si>
     <t>Invite teacher</t>
   </si>
   <si>
@@ -137,9 +121,6 @@
     <t>Search</t>
   </si>
   <si>
-    <t>Accept/Deny</t>
-  </si>
-  <si>
     <t>Accept/Deny an invitation</t>
   </si>
   <si>
@@ -167,9 +148,6 @@
     <t>Teachers manage students in their class</t>
   </si>
   <si>
-    <t>Manage website</t>
-  </si>
-  <si>
     <t>Manage users</t>
   </si>
   <si>
@@ -296,15 +274,9 @@
     <t>Design get forget password page</t>
   </si>
   <si>
-    <t>Pop-up form</t>
-  </si>
-  <si>
     <t>Create guest use-cases</t>
   </si>
   <si>
-    <t>Start after KhangTN commits overall usecase</t>
-  </si>
-  <si>
     <t>In process</t>
   </si>
   <si>
@@ -312,13 +284,100 @@
   </si>
   <si>
     <t>Waiting for Approval</t>
+  </si>
+  <si>
+    <t>Sprint 2</t>
+  </si>
+  <si>
+    <t>Design class page</t>
+  </si>
+  <si>
+    <t>Design post page</t>
+  </si>
+  <si>
+    <t>Design notification</t>
+  </si>
+  <si>
+    <t>Design teacher's profile viewer</t>
+  </si>
+  <si>
+    <t>Design student's profile viewer</t>
+  </si>
+  <si>
+    <t>Design invitation</t>
+  </si>
+  <si>
+    <t>Review use-case</t>
+  </si>
+  <si>
+    <t>Review conceptual diagram</t>
+  </si>
+  <si>
+    <t>Create guest use-case</t>
+  </si>
+  <si>
+    <t>Create teacher use-case</t>
+  </si>
+  <si>
+    <t>Create student use-case</t>
+  </si>
+  <si>
+    <t>Create admin use-case</t>
+  </si>
+  <si>
+    <t>Create system use-case</t>
+  </si>
+  <si>
+    <t>Create conceptual diagram</t>
+  </si>
+  <si>
+    <t>Start</t>
+  </si>
+  <si>
+    <t>End</t>
+  </si>
+  <si>
+    <t>19/5</t>
+  </si>
+  <si>
+    <t>25/5</t>
+  </si>
+  <si>
+    <t>Total task</t>
+  </si>
+  <si>
+    <t>Completed task</t>
+  </si>
+  <si>
+    <t>Not completed task</t>
+  </si>
+  <si>
+    <t>Review use-case, page design</t>
+  </si>
+  <si>
+    <t>Performance</t>
+  </si>
+  <si>
+    <t>Didn't meet deadline, didn't meet requirement</t>
+  </si>
+  <si>
+    <t>Didn't meet deadline</t>
+  </si>
+  <si>
+    <t>Start after KhangTN commits overall usecase, didn't submit</t>
+  </si>
+  <si>
+    <t>Didn't submit</t>
+  </si>
+  <si>
+    <t>Pop-up form, didn't submit</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -344,6 +403,13 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -359,7 +425,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -395,24 +461,11 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -426,17 +479,14 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -452,6 +502,306 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:dLbls>
+            <c:dLblPos val="ctr"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="1"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Sprint 1'!$B$38:$B$39</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>Completed task</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Not completed task</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sprint 1'!$C$38:$C$39</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="ctr"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
+        </c:dLbls>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Sprint 1'!$E$42</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Performance</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Sprint 1'!$B$43:$B$46</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>MinhKH</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>KhangTN</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>ThiTD</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>TungTD</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sprint 1'!$E$43:$E$46</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.25</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="50221568"/>
+        <c:axId val="49940160"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="50221568"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="49940160"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="49940160"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="0%" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="50221568"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>390525</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>219075</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="9" name="Chart 8"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -497,7 +847,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -532,7 +882,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -741,22 +1091,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D24"/>
+  <dimension ref="A1:C24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="1"/>
-    <col min="2" max="2" width="28.42578125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="32.7109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="100.85546875" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="1"/>
+    <col min="2" max="2" width="39.85546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="100.85546875" style="1" customWidth="1"/>
+    <col min="4" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="18" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -766,304 +1115,261 @@
       <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>1</v>
       </c>
-      <c r="B2" s="8" t="s">
-        <v>10</v>
+      <c r="B2" s="2" t="s">
+        <v>4</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>2</v>
       </c>
-      <c r="B3" s="8"/>
+      <c r="B3" s="2" t="s">
+        <v>3</v>
+      </c>
       <c r="C3" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>3</v>
       </c>
-      <c r="B4" s="8"/>
+      <c r="B4" s="2" t="s">
+        <v>7</v>
+      </c>
       <c r="C4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+        <v>30</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+        <v>9</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>6</v>
       </c>
-      <c r="B7" s="9" t="s">
+      <c r="B7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>7</v>
       </c>
-      <c r="B8" s="9"/>
+      <c r="B8" s="2" t="s">
+        <v>11</v>
+      </c>
       <c r="C8" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>8</v>
       </c>
-      <c r="B9" s="9" t="s">
-        <v>16</v>
+      <c r="B9" s="2" t="s">
+        <v>13</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>9</v>
       </c>
-      <c r="B10" s="9"/>
+      <c r="B10" s="2" t="s">
+        <v>15</v>
+      </c>
       <c r="C10" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>10</v>
       </c>
-      <c r="B11" s="9" t="s">
-        <v>38</v>
+      <c r="B11" s="2" t="s">
+        <v>34</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <v>11</v>
       </c>
-      <c r="B12" s="9"/>
+      <c r="B12" s="2" t="s">
+        <v>36</v>
+      </c>
       <c r="C12" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
         <v>12</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
         <v>13</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+        <v>40</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
         <v>14</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+        <v>39</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
         <v>15</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+        <v>19</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
         <v>16</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+        <v>20</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
         <v>17</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+        <v>21</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
         <v>18</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+        <v>24</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
         <v>19</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+        <v>26</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="2">
         <v>20</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+        <v>28</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="2">
         <v>21</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C22" s="2"/>
-      <c r="D22" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+        <v>33</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="2">
         <v>22</v>
       </c>
-      <c r="B23" s="10" t="s">
-        <v>48</v>
+      <c r="B23" s="2" t="s">
+        <v>43</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="2">
         <v>23</v>
       </c>
-      <c r="B24" s="11"/>
+      <c r="B24" s="2" t="s">
+        <v>44</v>
+      </c>
       <c r="C24" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="5">
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="B23:B24"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -1071,10 +1377,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M34"/>
+  <dimension ref="A1:M46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1090,7 +1396,7 @@
   <sheetData>
     <row r="1" spans="1:13" ht="25.5" x14ac:dyDescent="0.35">
       <c r="B1" s="4" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
@@ -1098,40 +1404,40 @@
         <v>0</v>
       </c>
       <c r="B3" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="G3" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="H3" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="D3" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="E3" s="5" t="s">
+      <c r="I3" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="J3" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="G3" s="5" t="s">
+      <c r="K3" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="L3" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="M3" s="5" t="s">
         <v>59</v>
-      </c>
-      <c r="H3" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="I3" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="J3" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="K3" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="L3" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="M3" s="5" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
@@ -1139,17 +1445,17 @@
         <v>1</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="2" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="E4" s="2">
         <v>10</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
@@ -1164,17 +1470,19 @@
         <v>2</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="C5" s="2"/>
+        <v>60</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>116</v>
+      </c>
       <c r="D5" s="2" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="E5" s="2">
         <v>6</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
@@ -1189,19 +1497,19 @@
         <v>3</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>91</v>
+        <v>117</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="E6" s="2">
         <v>6</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
@@ -1216,17 +1524,19 @@
         <v>4</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="C7" s="2"/>
+        <v>84</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>116</v>
+      </c>
       <c r="D7" s="2" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="E7" s="2">
         <v>6</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
@@ -1241,17 +1551,19 @@
         <v>5</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="C8" s="2"/>
+        <v>62</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>113</v>
+      </c>
       <c r="D8" s="2" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="E8" s="2">
         <v>8</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
@@ -1266,17 +1578,19 @@
         <v>6</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="C9" s="2"/>
+        <v>63</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>113</v>
+      </c>
       <c r="D9" s="2" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="E9" s="2">
         <v>8</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
@@ -1291,17 +1605,19 @@
         <v>7</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="C10" s="2"/>
+        <v>64</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>113</v>
+      </c>
       <c r="D10" s="2" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="E10" s="2">
         <v>8</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
@@ -1316,17 +1632,19 @@
         <v>8</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="C11" s="2"/>
+        <v>65</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>114</v>
+      </c>
       <c r="D11" s="2" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="E11" s="2">
         <v>4</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
@@ -1341,17 +1659,17 @@
         <v>9</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C12" s="2"/>
       <c r="D12" s="2" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="E12" s="2">
         <v>3</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
@@ -1366,17 +1684,17 @@
         <v>10</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" s="2" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="E13" s="2">
         <v>8</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
@@ -1391,17 +1709,17 @@
         <v>11</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="C14" s="2"/>
       <c r="D14" s="2" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="E14" s="2">
         <v>15</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
@@ -1416,19 +1734,19 @@
         <v>12</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>93</v>
+        <v>115</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="E15" s="2">
         <v>10</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
@@ -1440,20 +1758,20 @@
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="C16" s="2"/>
       <c r="D16" s="2" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="E16" s="2">
         <v>12</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
@@ -1465,20 +1783,20 @@
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="C17" s="2"/>
       <c r="D17" s="2" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="E17" s="2">
         <v>10</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
@@ -1490,20 +1808,22 @@
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="C18" s="2"/>
+        <v>71</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>114</v>
+      </c>
       <c r="D18" s="2" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="E18" s="2">
         <v>8</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
@@ -1515,20 +1835,20 @@
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="C19" s="2"/>
       <c r="D19" s="2" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="E19" s="2">
         <v>3</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
@@ -1538,109 +1858,799 @@
       <c r="L19" s="2"/>
       <c r="M19" s="2"/>
     </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A20" s="2">
+        <v>17</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E20" s="2">
+        <v>4</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="G20" s="2"/>
+      <c r="H20" s="2"/>
+      <c r="I20" s="2"/>
+      <c r="J20" s="2"/>
+      <c r="K20" s="2"/>
+      <c r="L20" s="2"/>
+      <c r="M20" s="2"/>
+    </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B22" s="1" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B23" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="C23" s="5" t="s">
-        <v>85</v>
+        <v>76</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B23" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="C23" s="11" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B24" s="2" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="C24" s="2">
-        <f>SUMIF(D4:D19,B24,E4:E19)</f>
-        <v>28</v>
+        <f>SUMIF(D4:D20,B24,E4:E20)</f>
+        <v>32</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B25" s="2" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="C25" s="2">
-        <f>SUMIF(D4:D19,B25,E4:E19)</f>
+        <f>SUMIF(D4:D20,B25,E4:E20)</f>
         <v>33</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B26" s="2" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="C26" s="2">
-        <f>SUMIF(D4:D19,B26,E4:E19)</f>
+        <f>SUMIF(D4:D20,B26,E4:E20)</f>
         <v>32</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B27" s="2" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="C27" s="2">
-        <f>SUMIF(D4:D19,B27,E4:E19)</f>
+        <f>SUMIF(D4:D20,B27,E4:E20)</f>
         <v>32</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B29" s="1" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B30" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="C30" s="5" t="s">
-        <v>85</v>
+        <v>81</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B30" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="C30" s="11" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B31" s="2" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="C31" s="2"/>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B32" s="2" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="C32" s="2"/>
     </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B33" s="2" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="C33" s="2"/>
     </row>
-    <row r="34" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B34" s="2" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="C34" s="2"/>
+    </row>
+    <row r="37" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B37" s="11" t="s">
+        <v>108</v>
+      </c>
+      <c r="C37" s="2">
+        <f>COUNTA(F4:F20)</f>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="38" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B38" s="11" t="s">
+        <v>109</v>
+      </c>
+      <c r="C38" s="2">
+        <f>COUNTIF(F4:F20,"Completed")</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="39" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B39" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="C39" s="2">
+        <f>C37-C38</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="42" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B42" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="C42" s="11" t="s">
+        <v>108</v>
+      </c>
+      <c r="D42" s="11" t="s">
+        <v>109</v>
+      </c>
+      <c r="E42" s="11" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="43" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B43" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C43" s="2">
+        <f>COUNTIF(D4:D20,B43)</f>
+        <v>5</v>
+      </c>
+      <c r="D43" s="2">
+        <v>5</v>
+      </c>
+      <c r="E43" s="12">
+        <f>D43/C43</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B44" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C44" s="2">
+        <f>COUNTIF(D4:D20,B44)</f>
+        <v>3</v>
+      </c>
+      <c r="D44" s="2">
+        <v>3</v>
+      </c>
+      <c r="E44" s="12">
+        <f t="shared" ref="E44:E46" si="0">D44/C44</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B45" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C45" s="2">
+        <f>COUNTIF(D4:D20,B45)</f>
+        <v>5</v>
+      </c>
+      <c r="D45" s="2">
+        <v>1</v>
+      </c>
+      <c r="E45" s="12">
+        <f t="shared" si="0"/>
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="46" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B46" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C46" s="2">
+        <f>COUNTIF(D4:D20,B46)</f>
+        <v>4</v>
+      </c>
+      <c r="D46" s="2">
+        <v>1</v>
+      </c>
+      <c r="E46" s="12">
+        <f t="shared" si="0"/>
+        <v>0.25</v>
+      </c>
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D4:D19">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D4:D20">
       <formula1>"MinhKH, KhangTN, ThiTD, TungTD"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F4:F19">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F4:F20">
       <formula1>"New, In process, Waiting for Approval, Completed"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <ignoredErrors>
-    <ignoredError sqref="C25" formula="1"/>
-  </ignoredErrors>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M34"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="1"/>
+    <col min="2" max="2" width="36.42578125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="17.85546875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="14.42578125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="18" style="1" customWidth="1"/>
+    <col min="6" max="6" width="21.7109375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="9.140625" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" ht="25.5" x14ac:dyDescent="0.35">
+      <c r="B1" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="I1" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A3" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="J3" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="K3" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="L3" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="M3" s="5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A4" s="2">
+        <v>1</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E4" s="2">
+        <v>12</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
+      <c r="L4" s="2"/>
+      <c r="M4" s="2"/>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A5" s="2">
+        <v>2</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E5" s="2">
+        <v>12</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
+      <c r="L5" s="2"/>
+      <c r="M5" s="2"/>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A6" s="2">
+        <v>3</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="E6" s="2">
+        <v>8</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
+      <c r="L6" s="2"/>
+      <c r="M6" s="2"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A7" s="2">
+        <v>4</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="E7" s="2">
+        <v>8</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2"/>
+      <c r="L7" s="2"/>
+      <c r="M7" s="2"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A8" s="2">
+        <v>5</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="E8" s="2">
+        <v>8</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2"/>
+      <c r="L8" s="2"/>
+      <c r="M8" s="2"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A9" s="2">
+        <v>6</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="E9" s="2">
+        <v>8</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="2"/>
+      <c r="L9" s="2"/>
+      <c r="M9" s="2"/>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A10" s="2">
+        <v>7</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="E10" s="2">
+        <v>10</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
+      <c r="J10" s="2"/>
+      <c r="K10" s="2"/>
+      <c r="L10" s="2"/>
+      <c r="M10" s="2"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A11" s="2">
+        <v>8</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="E11" s="2">
+        <v>16</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
+      <c r="I11" s="2"/>
+      <c r="J11" s="2"/>
+      <c r="K11" s="2"/>
+      <c r="L11" s="2"/>
+      <c r="M11" s="2"/>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A12" s="2">
+        <v>9</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="E12" s="2">
+        <v>16</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2"/>
+      <c r="J12" s="2"/>
+      <c r="K12" s="2"/>
+      <c r="L12" s="2"/>
+      <c r="M12" s="2"/>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A13" s="2">
+        <v>10</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="E13" s="2">
+        <v>8</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
+      <c r="I13" s="2"/>
+      <c r="J13" s="2"/>
+      <c r="K13" s="2"/>
+      <c r="L13" s="2"/>
+      <c r="M13" s="2"/>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A14" s="2">
+        <v>11</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="E14" s="2">
+        <v>8</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
+      <c r="I14" s="2"/>
+      <c r="J14" s="2"/>
+      <c r="K14" s="2"/>
+      <c r="L14" s="2"/>
+      <c r="M14" s="2"/>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A15" s="2">
+        <v>12</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="E15" s="2">
+        <v>6</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2"/>
+      <c r="I15" s="2"/>
+      <c r="J15" s="2"/>
+      <c r="K15" s="2"/>
+      <c r="L15" s="2"/>
+      <c r="M15" s="2"/>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A16" s="2">
+        <v>12</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E16" s="2">
+        <v>6</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="G16" s="2"/>
+      <c r="H16" s="2"/>
+      <c r="I16" s="2"/>
+      <c r="J16" s="2"/>
+      <c r="K16" s="2"/>
+      <c r="L16" s="2"/>
+      <c r="M16" s="2"/>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A17" s="2">
+        <v>13</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E17" s="2">
+        <v>4</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="G17" s="2"/>
+      <c r="H17" s="2"/>
+      <c r="I17" s="2"/>
+      <c r="J17" s="2"/>
+      <c r="K17" s="2"/>
+      <c r="L17" s="2"/>
+      <c r="M17" s="2"/>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A18" s="2">
+        <v>14</v>
+      </c>
+      <c r="B18" s="9"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+      <c r="H18" s="2"/>
+      <c r="I18" s="2"/>
+      <c r="J18" s="2"/>
+      <c r="K18" s="2"/>
+      <c r="L18" s="2"/>
+      <c r="M18" s="2"/>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A19" s="2">
+        <v>15</v>
+      </c>
+      <c r="B19" s="2"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+      <c r="G19" s="2"/>
+      <c r="H19" s="2"/>
+      <c r="I19" s="2"/>
+      <c r="J19" s="2"/>
+      <c r="K19" s="2"/>
+      <c r="L19" s="2"/>
+      <c r="M19" s="2"/>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B22" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B23" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B24" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C24" s="2">
+        <f>SUMIF(D4:D19,B24,E4:E19)</f>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B25" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C25" s="2">
+        <f>SUMIF(D4:D19,B25,E4:E19)</f>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B26" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C26" s="2">
+        <f>SUMIF(D4:D19,B26,E4:E19)</f>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B27" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C27" s="2">
+        <f>SUMIF(D4:D19,B27,E4:E19)</f>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B29" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B30" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B31" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C31" s="2"/>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B32" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C32" s="2"/>
+    </row>
+    <row r="33" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B33" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C33" s="2"/>
+    </row>
+    <row r="34" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B34" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C34" s="2"/>
+    </row>
+  </sheetData>
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F4:F19">
+      <formula1>"New, In process, Waiting for Approval, Completed"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D4:D19">
+      <formula1>"MinhKH, KhangTN, ThiTD, TungTD"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>

<commit_message>
Submit Use case specification, update Backlog
</commit_message>
<xml_diff>
--- a/QA Backlog.xlsx
+++ b/QA Backlog.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="97">
   <si>
     <t>No</t>
   </si>
@@ -24,6 +24,9 @@
     <t>Function</t>
   </si>
   <si>
+    <t>Detail</t>
+  </si>
+  <si>
     <t>Description</t>
   </si>
   <si>
@@ -42,9 +45,18 @@
     <t>Get forgotton password</t>
   </si>
   <si>
+    <t>Reseting password if forgetting</t>
+  </si>
+  <si>
+    <t>Autheticate</t>
+  </si>
+  <si>
     <t>Create class</t>
   </si>
   <si>
+    <t>Create post</t>
+  </si>
+  <si>
     <t>Create article, question, answer</t>
   </si>
   <si>
@@ -54,6 +66,9 @@
     <t>User post an article, ask a question or answer a question</t>
   </si>
   <si>
+    <t>Invite user</t>
+  </si>
+  <si>
     <t>Invite teacher</t>
   </si>
   <si>
@@ -117,6 +132,9 @@
     <t>Search</t>
   </si>
   <si>
+    <t>Accept/Deny</t>
+  </si>
+  <si>
     <t>Accept/Deny an invitation</t>
   </si>
   <si>
@@ -144,12 +162,21 @@
     <t>Teachers manage students in their class</t>
   </si>
   <si>
+    <t>Manage website</t>
+  </si>
+  <si>
     <t>Manage users</t>
   </si>
   <si>
+    <t>Manage psots</t>
+  </si>
+  <si>
     <t>Admin can ban/unban users</t>
   </si>
   <si>
+    <t>Admin can remove posts</t>
+  </si>
+  <si>
     <t>Task</t>
   </si>
   <si>
@@ -270,6 +297,9 @@
     <t>Create guest use-cases</t>
   </si>
   <si>
+    <t>Start after KhangTN commits overall usecase</t>
+  </si>
+  <si>
     <t>In process</t>
   </si>
   <si>
@@ -277,28 +307,13 @@
   </si>
   <si>
     <t>Waiting for Approval</t>
-  </si>
-  <si>
-    <t>Resetting password if forgetting</t>
-  </si>
-  <si>
-    <t>Added in sprint</t>
-  </si>
-  <si>
-    <t>not commit at deadline</t>
-  </si>
-  <si>
-    <t>Start after KhangTN commits overall usecase, not commit at deadline</t>
-  </si>
-  <si>
-    <t>Review Use-case, UI design</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -324,18 +339,6 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FFFF0000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="4" tint="-0.249977111117893"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -351,7 +354,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -387,6 +390,19 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -401,13 +417,21 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -712,18 +736,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D23"/>
+  <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="1"/>
     <col min="2" max="2" width="28.42578125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="100.85546875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="19.28515625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="32.7109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="100.85546875" style="1" customWidth="1"/>
     <col min="5" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
@@ -738,274 +762,303 @@
         <v>2</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>88</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>4</v>
+      <c r="B2" s="8" t="s">
+        <v>10</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="2"/>
+        <v>5</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>2</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>3</v>
-      </c>
+      <c r="B3" s="8"/>
       <c r="C3" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" s="2"/>
+        <v>4</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>3</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>7</v>
-      </c>
+      <c r="B4" s="8"/>
       <c r="C4" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="D4" s="2"/>
+        <v>8</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="D5" s="2"/>
+        <v>34</v>
+      </c>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="D6" s="2"/>
+        <v>11</v>
+      </c>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>6</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>9</v>
+      <c r="B7" s="9" t="s">
+        <v>12</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D7" s="2"/>
+        <v>13</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>7</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>10</v>
-      </c>
+      <c r="B8" s="9"/>
       <c r="C8" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D8" s="2"/>
+        <v>14</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>8</v>
       </c>
-      <c r="B9" s="2" t="s">
-        <v>12</v>
+      <c r="B9" s="9" t="s">
+        <v>16</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D9" s="2"/>
+        <v>17</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>9</v>
       </c>
-      <c r="B10" s="2" t="s">
-        <v>14</v>
-      </c>
+      <c r="B10" s="9"/>
       <c r="C10" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D10" s="2"/>
+        <v>19</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>10</v>
       </c>
-      <c r="B11" s="2" t="s">
-        <v>33</v>
+      <c r="B11" s="9" t="s">
+        <v>38</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="D11" s="2"/>
+        <v>39</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <v>11</v>
       </c>
-      <c r="B12" s="2" t="s">
-        <v>35</v>
-      </c>
+      <c r="B12" s="9"/>
       <c r="C12" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="D12" s="2"/>
+        <v>41</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
         <v>12</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D13" s="2"/>
+        <v>22</v>
+      </c>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
         <v>13</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="D14" s="2"/>
+        <v>45</v>
+      </c>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
         <v>14</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="D15" s="2"/>
+        <v>44</v>
+      </c>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
         <v>15</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="D16" s="2"/>
+        <v>23</v>
+      </c>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
         <v>16</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="D17" s="2"/>
+        <v>24</v>
+      </c>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
         <v>17</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D18" s="2"/>
+        <v>25</v>
+      </c>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
         <v>18</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D19" s="2"/>
+        <v>28</v>
+      </c>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
         <v>19</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="D20" s="2"/>
+        <v>30</v>
+      </c>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="2">
         <v>20</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="D21" s="2"/>
+        <v>32</v>
+      </c>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="2">
         <v>21</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C22" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="D22" s="2"/>
+      <c r="C22" s="2"/>
+      <c r="D22" s="2" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="2">
         <v>22</v>
       </c>
-      <c r="B23" s="2" t="s">
-        <v>42</v>
+      <c r="B23" s="10" t="s">
+        <v>48</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="D23" s="2"/>
+        <v>49</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" s="2">
+        <v>23</v>
+      </c>
+      <c r="B24" s="11"/>
+      <c r="C24" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>52</v>
+      </c>
     </row>
   </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="B23:B24"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -1016,14 +1069,14 @@
   <dimension ref="A1:M34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="1"/>
     <col min="2" max="2" width="36.42578125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="25.28515625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="17.85546875" style="1" customWidth="1"/>
     <col min="4" max="4" width="14.42578125" style="1" customWidth="1"/>
     <col min="5" max="5" width="18" style="1" customWidth="1"/>
     <col min="6" max="6" width="21.7109375" style="1" customWidth="1"/>
@@ -1032,7 +1085,7 @@
   <sheetData>
     <row r="1" spans="1:13" ht="25.5" x14ac:dyDescent="0.35">
       <c r="B1" s="4" t="s">
-        <v>74</v>
+        <v>83</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
@@ -1040,40 +1093,40 @@
         <v>0</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>45</v>
+        <v>54</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>75</v>
+        <v>84</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>50</v>
+        <v>59</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>51</v>
+        <v>60</v>
       </c>
       <c r="I3" s="5" t="s">
-        <v>52</v>
+        <v>61</v>
       </c>
       <c r="J3" s="5" t="s">
-        <v>53</v>
+        <v>62</v>
       </c>
       <c r="K3" s="5" t="s">
-        <v>54</v>
+        <v>63</v>
       </c>
       <c r="L3" s="5" t="s">
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="M3" s="5" t="s">
-        <v>56</v>
+        <v>65</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
@@ -1081,17 +1134,17 @@
         <v>1</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>48</v>
+        <v>57</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="2" t="s">
-        <v>49</v>
+        <v>58</v>
       </c>
       <c r="E4" s="2">
         <v>10</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>85</v>
+        <v>94</v>
       </c>
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
@@ -1101,186 +1154,174 @@
       <c r="L4" s="2"/>
       <c r="M4" s="2"/>
     </row>
-    <row r="5" spans="1:13" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="7">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A5" s="2">
         <v>2</v>
       </c>
-      <c r="B5" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>89</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="E5" s="7">
+      <c r="B5" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="E5" s="2">
         <v>6</v>
       </c>
-      <c r="F5" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="G5" s="7"/>
-      <c r="H5" s="7"/>
-      <c r="I5" s="7"/>
-      <c r="J5" s="7"/>
-      <c r="K5" s="7"/>
-      <c r="L5" s="7"/>
-      <c r="M5" s="7"/>
-    </row>
-    <row r="6" spans="1:13" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="7">
+      <c r="F5" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
+      <c r="L5" s="2"/>
+      <c r="M5" s="2"/>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A6" s="2">
         <v>3</v>
       </c>
-      <c r="B6" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="E6" s="7">
+      <c r="B6" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="E6" s="2">
         <v>6</v>
       </c>
-      <c r="F6" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="G6" s="7"/>
-      <c r="H6" s="7"/>
-      <c r="I6" s="7"/>
-      <c r="J6" s="7"/>
-      <c r="K6" s="7"/>
-      <c r="L6" s="7"/>
-      <c r="M6" s="7"/>
-    </row>
-    <row r="7" spans="1:13" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="7">
+      <c r="F6" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
+      <c r="L6" s="2"/>
+      <c r="M6" s="2"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A7" s="2">
         <v>4</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="E7" s="2">
+        <v>6</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2"/>
+      <c r="L7" s="2"/>
+      <c r="M7" s="2"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A8" s="2">
+        <v>5</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="C7" s="7" t="s">
-        <v>89</v>
-      </c>
-      <c r="D7" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="E7" s="7">
+      <c r="E8" s="2">
+        <v>8</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2"/>
+      <c r="L8" s="2"/>
+      <c r="M8" s="2"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A9" s="2">
         <v>6</v>
       </c>
-      <c r="F7" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="G7" s="7"/>
-      <c r="H7" s="7"/>
-      <c r="I7" s="7"/>
-      <c r="J7" s="7"/>
-      <c r="K7" s="7"/>
-      <c r="L7" s="7"/>
-      <c r="M7" s="7"/>
-    </row>
-    <row r="8" spans="1:13" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="7">
-        <v>5</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>89</v>
-      </c>
-      <c r="D8" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="E8" s="7">
+      <c r="B9" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="E9" s="2">
         <v>8</v>
       </c>
-      <c r="F8" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="G8" s="7"/>
-      <c r="H8" s="7"/>
-      <c r="I8" s="7"/>
-      <c r="J8" s="7"/>
-      <c r="K8" s="7"/>
-      <c r="L8" s="7"/>
-      <c r="M8" s="7"/>
-    </row>
-    <row r="9" spans="1:13" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="7">
-        <v>6</v>
-      </c>
-      <c r="B9" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>89</v>
-      </c>
-      <c r="D9" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="E9" s="7">
+      <c r="F9" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="2"/>
+      <c r="L9" s="2"/>
+      <c r="M9" s="2"/>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A10" s="2">
+        <v>7</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="E10" s="2">
         <v>8</v>
       </c>
-      <c r="F9" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="G9" s="7"/>
-      <c r="H9" s="7"/>
-      <c r="I9" s="7"/>
-      <c r="J9" s="7"/>
-      <c r="K9" s="7"/>
-      <c r="L9" s="7"/>
-      <c r="M9" s="7"/>
-    </row>
-    <row r="10" spans="1:13" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="7">
-        <v>7</v>
-      </c>
-      <c r="B10" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="C10" s="7" t="s">
-        <v>89</v>
-      </c>
-      <c r="D10" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="E10" s="7">
-        <v>8</v>
-      </c>
-      <c r="F10" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="G10" s="7"/>
-      <c r="H10" s="7"/>
-      <c r="I10" s="7"/>
-      <c r="J10" s="7"/>
-      <c r="K10" s="7"/>
-      <c r="L10" s="7"/>
-      <c r="M10" s="7"/>
+      <c r="F10" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
+      <c r="J10" s="2"/>
+      <c r="K10" s="2"/>
+      <c r="L10" s="2"/>
+      <c r="M10" s="2"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>8</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>89</v>
-      </c>
+        <v>71</v>
+      </c>
+      <c r="C11" s="2"/>
       <c r="D11" s="2" t="s">
-        <v>71</v>
+        <v>80</v>
       </c>
       <c r="E11" s="2">
         <v>4</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>85</v>
+        <v>95</v>
       </c>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
@@ -1295,17 +1336,17 @@
         <v>9</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>63</v>
+        <v>72</v>
       </c>
       <c r="C12" s="2"/>
       <c r="D12" s="2" t="s">
-        <v>49</v>
+        <v>58</v>
       </c>
       <c r="E12" s="2">
         <v>3</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>85</v>
+        <v>95</v>
       </c>
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
@@ -1320,17 +1361,17 @@
         <v>10</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>64</v>
+        <v>73</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" s="2" t="s">
-        <v>70</v>
+        <v>79</v>
       </c>
       <c r="E13" s="2">
         <v>8</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>85</v>
+        <v>96</v>
       </c>
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
@@ -1345,17 +1386,17 @@
         <v>11</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>65</v>
+        <v>74</v>
       </c>
       <c r="C14" s="2"/>
       <c r="D14" s="2" t="s">
-        <v>70</v>
+        <v>79</v>
       </c>
       <c r="E14" s="2">
         <v>15</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>85</v>
+        <v>95</v>
       </c>
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
@@ -1365,49 +1406,49 @@
       <c r="L14" s="2"/>
       <c r="M14" s="2"/>
     </row>
-    <row r="15" spans="1:13" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="7">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A15" s="2">
         <v>12</v>
       </c>
-      <c r="B15" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="C15" s="7" t="s">
-        <v>90</v>
-      </c>
-      <c r="D15" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="E15" s="7">
+      <c r="B15" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="E15" s="2">
         <v>10</v>
       </c>
-      <c r="F15" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="G15" s="7"/>
-      <c r="H15" s="7"/>
-      <c r="I15" s="7"/>
-      <c r="J15" s="7"/>
-      <c r="K15" s="7"/>
-      <c r="L15" s="7"/>
-      <c r="M15" s="7"/>
+      <c r="F15" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2"/>
+      <c r="I15" s="2"/>
+      <c r="J15" s="2"/>
+      <c r="K15" s="2"/>
+      <c r="L15" s="2"/>
+      <c r="M15" s="2"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>66</v>
+        <v>75</v>
       </c>
       <c r="C16" s="2"/>
       <c r="D16" s="2" t="s">
-        <v>49</v>
+        <v>58</v>
       </c>
       <c r="E16" s="2">
         <v>12</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>85</v>
+        <v>95</v>
       </c>
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
@@ -1419,20 +1460,20 @@
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>67</v>
+        <v>76</v>
       </c>
       <c r="C17" s="2"/>
       <c r="D17" s="2" t="s">
-        <v>70</v>
+        <v>79</v>
       </c>
       <c r="E17" s="2">
         <v>10</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>86</v>
+        <v>96</v>
       </c>
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
@@ -1442,49 +1483,47 @@
       <c r="L17" s="2"/>
       <c r="M17" s="2"/>
     </row>
-    <row r="18" spans="1:13" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="9">
-        <v>15</v>
-      </c>
-      <c r="B18" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="C18" s="9" t="s">
-        <v>89</v>
-      </c>
-      <c r="D18" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="E18" s="9">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A18" s="2">
+        <v>14</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="E18" s="2">
         <v>8</v>
       </c>
-      <c r="F18" s="9" t="s">
-        <v>85</v>
-      </c>
-      <c r="G18" s="9"/>
-      <c r="H18" s="9"/>
-      <c r="I18" s="9"/>
-      <c r="J18" s="9"/>
-      <c r="K18" s="9"/>
-      <c r="L18" s="9"/>
-      <c r="M18" s="9"/>
+      <c r="F18" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="G18" s="2"/>
+      <c r="H18" s="2"/>
+      <c r="I18" s="2"/>
+      <c r="J18" s="2"/>
+      <c r="K18" s="2"/>
+      <c r="L18" s="2"/>
+      <c r="M18" s="2"/>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>69</v>
+        <v>78</v>
       </c>
       <c r="C19" s="2"/>
       <c r="D19" s="2" t="s">
-        <v>49</v>
+        <v>58</v>
       </c>
       <c r="E19" s="2">
         <v>3</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
@@ -1494,114 +1533,89 @@
       <c r="L19" s="2"/>
       <c r="M19" s="2"/>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A20" s="2">
-        <v>17</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="E20" s="2">
-        <v>4</v>
-      </c>
-      <c r="F20" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="G20" s="2"/>
-      <c r="H20" s="2"/>
-      <c r="I20" s="2"/>
-      <c r="J20" s="2"/>
-      <c r="K20" s="2"/>
-      <c r="L20" s="2"/>
-      <c r="M20" s="2"/>
-    </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B22" s="1" t="s">
-        <v>73</v>
+        <v>82</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B23" s="5" t="s">
-        <v>75</v>
+        <v>84</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>76</v>
+        <v>85</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B24" s="2" t="s">
-        <v>49</v>
+        <v>58</v>
       </c>
       <c r="C24" s="2">
-        <f>SUMIF(D4:D20,B24,E4:E20)</f>
-        <v>32</v>
+        <f>SUMIF(D4:D19,B24,E4:E19)</f>
+        <v>28</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B25" s="2" t="s">
-        <v>70</v>
+        <v>79</v>
       </c>
       <c r="C25" s="2">
-        <f>SUMIF(D4:D20,B25,E4:E20)</f>
+        <f>SUMIF(D4:D19,B25,E4:E19)</f>
         <v>33</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B26" s="2" t="s">
-        <v>71</v>
+        <v>80</v>
       </c>
       <c r="C26" s="2">
-        <f>SUMIF(D4:D20,B26,E4:E20)</f>
+        <f>SUMIF(D4:D19,B26,E4:E19)</f>
         <v>32</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B27" s="2" t="s">
-        <v>72</v>
+        <v>81</v>
       </c>
       <c r="C27" s="2">
-        <f>SUMIF(D4:D20,B27,E4:E20)</f>
+        <f>SUMIF(D4:D19,B27,E4:E19)</f>
         <v>32</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B29" s="1" t="s">
-        <v>78</v>
+        <v>87</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B30" s="5" t="s">
-        <v>75</v>
+        <v>84</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>76</v>
+        <v>85</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B31" s="2" t="s">
-        <v>49</v>
+        <v>58</v>
       </c>
       <c r="C31" s="2"/>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B32" s="2" t="s">
-        <v>70</v>
+        <v>79</v>
       </c>
       <c r="C32" s="2"/>
     </row>
     <row r="33" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B33" s="2" t="s">
-        <v>71</v>
+        <v>80</v>
       </c>
       <c r="C33" s="2"/>
     </row>
     <row r="34" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B34" s="2" t="s">
-        <v>72</v>
+        <v>81</v>
       </c>
       <c r="C34" s="2"/>
     </row>
@@ -1610,12 +1624,14 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D4:D19">
       <formula1>"MinhKH, KhangTN, ThiTD, TungTD"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F4:F20">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F4:F19">
       <formula1>"New, In process, Waiting for Approval, Completed"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <ignoredErrors>
+    <ignoredError sqref="C25" formula="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Update backlog sprint 1
</commit_message>
<xml_diff>
--- a/QA Backlog.xlsx
+++ b/QA Backlog.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="117">
   <si>
     <t>No</t>
   </si>
@@ -281,9 +281,6 @@
   </si>
   <si>
     <t>Completed</t>
-  </si>
-  <si>
-    <t>Waiting for Approval</t>
   </si>
   <si>
     <t>Sprint 2</t>
@@ -377,7 +374,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -410,8 +407,14 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -421,6 +424,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -465,7 +474,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -487,6 +496,8 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -611,6 +622,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -686,11 +698,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="50221568"/>
-        <c:axId val="49940160"/>
+        <c:axId val="54194688"/>
+        <c:axId val="70867712"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="50221568"/>
+        <c:axId val="54194688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -699,7 +711,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="49940160"/>
+        <c:crossAx val="70867712"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -707,7 +719,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="49940160"/>
+        <c:axId val="70867712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -718,13 +730,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="50221568"/>
+        <c:crossAx val="54194688"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1380,7 +1393,7 @@
   <dimension ref="A1:M46"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1465,167 +1478,167 @@
       <c r="L4" s="2"/>
       <c r="M4" s="2"/>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A5" s="2">
+    <row r="5" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="13">
         <v>2</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="13" t="s">
+        <v>115</v>
+      </c>
+      <c r="D5" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="E5" s="13">
+        <v>6</v>
+      </c>
+      <c r="F5" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="G5" s="13"/>
+      <c r="H5" s="13"/>
+      <c r="I5" s="13"/>
+      <c r="J5" s="13"/>
+      <c r="K5" s="13"/>
+      <c r="L5" s="13"/>
+      <c r="M5" s="13"/>
+    </row>
+    <row r="6" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="13">
+        <v>3</v>
+      </c>
+      <c r="B6" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="C6" s="13" t="s">
         <v>116</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D6" s="13" t="s">
         <v>74</v>
       </c>
-      <c r="E5" s="2">
+      <c r="E6" s="13">
         <v>6</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="F6" s="13" t="s">
         <v>86</v>
       </c>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
-      <c r="J5" s="2"/>
-      <c r="K5" s="2"/>
-      <c r="L5" s="2"/>
-      <c r="M5" s="2"/>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A6" s="2">
-        <v>3</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="D6" s="2" t="s">
+      <c r="G6" s="13"/>
+      <c r="H6" s="13"/>
+      <c r="I6" s="13"/>
+      <c r="J6" s="13"/>
+      <c r="K6" s="13"/>
+      <c r="L6" s="13"/>
+      <c r="M6" s="13"/>
+    </row>
+    <row r="7" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="13">
+        <v>4</v>
+      </c>
+      <c r="B7" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="C7" s="13" t="s">
+        <v>115</v>
+      </c>
+      <c r="D7" s="13" t="s">
         <v>74</v>
       </c>
-      <c r="E6" s="2">
+      <c r="E7" s="13">
         <v>6</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="F7" s="13" t="s">
         <v>86</v>
       </c>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
-      <c r="J6" s="2"/>
-      <c r="K6" s="2"/>
-      <c r="L6" s="2"/>
-      <c r="M6" s="2"/>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A7" s="2">
-        <v>4</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="E7" s="2">
+      <c r="G7" s="13"/>
+      <c r="H7" s="13"/>
+      <c r="I7" s="13"/>
+      <c r="J7" s="13"/>
+      <c r="K7" s="13"/>
+      <c r="L7" s="13"/>
+      <c r="M7" s="13"/>
+    </row>
+    <row r="8" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="13">
+        <v>5</v>
+      </c>
+      <c r="B8" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="C8" s="13" t="s">
+        <v>112</v>
+      </c>
+      <c r="D8" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="E8" s="13">
+        <v>8</v>
+      </c>
+      <c r="F8" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="G8" s="13"/>
+      <c r="H8" s="13"/>
+      <c r="I8" s="13"/>
+      <c r="J8" s="13"/>
+      <c r="K8" s="13"/>
+      <c r="L8" s="13"/>
+      <c r="M8" s="13"/>
+    </row>
+    <row r="9" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="13">
         <v>6</v>
       </c>
-      <c r="F7" s="2" t="s">
+      <c r="B9" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="C9" s="13" t="s">
+        <v>112</v>
+      </c>
+      <c r="D9" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="E9" s="13">
+        <v>8</v>
+      </c>
+      <c r="F9" s="13" t="s">
         <v>86</v>
       </c>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
-      <c r="I7" s="2"/>
-      <c r="J7" s="2"/>
-      <c r="K7" s="2"/>
-      <c r="L7" s="2"/>
-      <c r="M7" s="2"/>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A8" s="2">
-        <v>5</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="D8" s="2" t="s">
+      <c r="G9" s="13"/>
+      <c r="H9" s="13"/>
+      <c r="I9" s="13"/>
+      <c r="J9" s="13"/>
+      <c r="K9" s="13"/>
+      <c r="L9" s="13"/>
+      <c r="M9" s="13"/>
+    </row>
+    <row r="10" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="13">
+        <v>7</v>
+      </c>
+      <c r="B10" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="C10" s="13" t="s">
+        <v>112</v>
+      </c>
+      <c r="D10" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="E8" s="2">
+      <c r="E10" s="13">
         <v>8</v>
       </c>
-      <c r="F8" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
-      <c r="I8" s="2"/>
-      <c r="J8" s="2"/>
-      <c r="K8" s="2"/>
-      <c r="L8" s="2"/>
-      <c r="M8" s="2"/>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A9" s="2">
-        <v>6</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="E9" s="2">
-        <v>8</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
-      <c r="I9" s="2"/>
-      <c r="J9" s="2"/>
-      <c r="K9" s="2"/>
-      <c r="L9" s="2"/>
-      <c r="M9" s="2"/>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A10" s="2">
-        <v>7</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="E10" s="2">
-        <v>8</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
-      <c r="I10" s="2"/>
-      <c r="J10" s="2"/>
-      <c r="K10" s="2"/>
-      <c r="L10" s="2"/>
-      <c r="M10" s="2"/>
+      <c r="F10" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="G10" s="13"/>
+      <c r="H10" s="13"/>
+      <c r="I10" s="13"/>
+      <c r="J10" s="13"/>
+      <c r="K10" s="13"/>
+      <c r="L10" s="13"/>
+      <c r="M10" s="13"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
@@ -1635,7 +1648,7 @@
         <v>65</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>74</v>
@@ -1729,32 +1742,32 @@
       <c r="L14" s="2"/>
       <c r="M14" s="2"/>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A15" s="2">
+    <row r="15" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="13">
         <v>12</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B15" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="C15" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="D15" s="2" t="s">
+      <c r="C15" s="13" t="s">
+        <v>114</v>
+      </c>
+      <c r="D15" s="13" t="s">
         <v>74</v>
       </c>
-      <c r="E15" s="2">
+      <c r="E15" s="13">
         <v>10</v>
       </c>
-      <c r="F15" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="G15" s="2"/>
-      <c r="H15" s="2"/>
-      <c r="I15" s="2"/>
-      <c r="J15" s="2"/>
-      <c r="K15" s="2"/>
-      <c r="L15" s="2"/>
-      <c r="M15" s="2"/>
+      <c r="F15" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="G15" s="13"/>
+      <c r="H15" s="13"/>
+      <c r="I15" s="13"/>
+      <c r="J15" s="13"/>
+      <c r="K15" s="13"/>
+      <c r="L15" s="13"/>
+      <c r="M15" s="13"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
@@ -1814,7 +1827,7 @@
         <v>71</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>75</v>
@@ -1863,7 +1876,7 @@
         <v>17</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C20" s="2"/>
       <c r="D20" s="2" t="s">
@@ -1971,7 +1984,7 @@
     </row>
     <row r="37" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B37" s="11" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C37" s="2">
         <f>COUNTA(F4:F20)</f>
@@ -1980,7 +1993,7 @@
     </row>
     <row r="38" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B38" s="11" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C38" s="2">
         <f>COUNTIF(F4:F20,"Completed")</f>
@@ -1989,7 +2002,7 @@
     </row>
     <row r="39" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B39" s="11" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C39" s="2">
         <f>C37-C38</f>
@@ -2001,13 +2014,13 @@
         <v>78</v>
       </c>
       <c r="C42" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="D42" s="11" t="s">
         <v>108</v>
       </c>
-      <c r="D42" s="11" t="s">
-        <v>109</v>
-      </c>
       <c r="E42" s="11" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="43" spans="2:5" x14ac:dyDescent="0.2">
@@ -2084,7 +2097,8 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -2110,19 +2124,19 @@
   <sheetData>
     <row r="1" spans="1:13" ht="25.5" x14ac:dyDescent="0.35">
       <c r="B1" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G1" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="I1" s="10" t="s">
         <v>104</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>106</v>
-      </c>
-      <c r="I1" s="10" t="s">
-        <v>105</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
@@ -2171,7 +2185,7 @@
         <v>1</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="2" t="s">
@@ -2196,7 +2210,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C5" s="2"/>
       <c r="D5" s="2" t="s">
@@ -2221,7 +2235,7 @@
         <v>3</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C6" s="2"/>
       <c r="D6" s="2" t="s">
@@ -2246,7 +2260,7 @@
         <v>4</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="2" t="s">
@@ -2271,7 +2285,7 @@
         <v>5</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C8" s="2"/>
       <c r="D8" s="2" t="s">
@@ -2296,7 +2310,7 @@
         <v>6</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="2" t="s">
@@ -2321,7 +2335,7 @@
         <v>7</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C10" s="2"/>
       <c r="D10" s="2" t="s">
@@ -2346,7 +2360,7 @@
         <v>8</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C11" s="2"/>
       <c r="D11" s="2" t="s">
@@ -2371,7 +2385,7 @@
         <v>9</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C12" s="2"/>
       <c r="D12" s="2" t="s">
@@ -2396,7 +2410,7 @@
         <v>10</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" s="2" t="s">
@@ -2421,7 +2435,7 @@
         <v>11</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C14" s="2"/>
       <c r="D14" s="2" t="s">
@@ -2446,7 +2460,7 @@
         <v>12</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C15" s="2"/>
       <c r="D15" s="2" t="s">
@@ -2471,7 +2485,7 @@
         <v>12</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C16" s="2"/>
       <c r="D16" s="2" t="s">
@@ -2496,7 +2510,7 @@
         <v>13</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C17" s="2"/>
       <c r="D17" s="2" t="s">

</xml_diff>

<commit_message>
update sprint 2 minhkh
</commit_message>
<xml_diff>
--- a/QA Backlog.xlsx
+++ b/QA Backlog.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\study\Capstone\Document\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="240" yWindow="60" windowWidth="20115" windowHeight="8010" activeTab="1"/>
   </bookViews>
@@ -15,9 +10,9 @@
     <sheet name="Product Backlog" sheetId="1" r:id="rId1"/>
     <sheet name="Sprint 1" sheetId="2" r:id="rId2"/>
     <sheet name="Sprint 2" sheetId="4" r:id="rId3"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId4"/>
+    <sheet name="Sprint 3" sheetId="3" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="152511" concurrentCalc="0"/>
+  <calcPr calcId="144525" concurrentCalc="0"/>
 </workbook>
 </file>
 
@@ -723,11 +718,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="200664256"/>
-        <c:axId val="200639120"/>
+        <c:axId val="64979456"/>
+        <c:axId val="64833216"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="200664256"/>
+        <c:axId val="64979456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -737,7 +732,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="200639120"/>
+        <c:crossAx val="64833216"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -745,7 +740,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="200639120"/>
+        <c:axId val="64833216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -756,7 +751,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="200664256"/>
+        <c:crossAx val="64979456"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -886,7 +881,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -921,7 +916,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2161,7 +2156,7 @@
   <dimension ref="A1:M39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2249,7 +2244,7 @@
         <v>12</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
@@ -2877,7 +2872,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>

</xml_diff>

<commit_message>
Update backlog task sprint 2
</commit_message>
<xml_diff>
--- a/QA Backlog.xlsx
+++ b/QA Backlog.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="116">
   <si>
     <t>No</t>
   </si>
@@ -362,6 +362,9 @@
   </si>
   <si>
     <t>Fix System architecture</t>
+  </si>
+  <si>
+    <t>Sprint 1 task (ThiTD -&gt; MinhKH)</t>
   </si>
 </sst>
 </file>
@@ -2142,7 +2145,7 @@
   <dimension ref="A1:M37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2398,7 +2401,7 @@
         <v>60</v>
       </c>
       <c r="C11" s="13" t="s">
-        <v>108</v>
+        <v>115</v>
       </c>
       <c r="D11" s="14" t="s">
         <v>52</v>
@@ -2425,7 +2428,7 @@
         <v>61</v>
       </c>
       <c r="C12" s="13" t="s">
-        <v>108</v>
+        <v>115</v>
       </c>
       <c r="D12" s="14" t="s">
         <v>52</v>
@@ -2452,7 +2455,7 @@
         <v>84</v>
       </c>
       <c r="C13" s="13" t="s">
-        <v>108</v>
+        <v>115</v>
       </c>
       <c r="D13" s="14" t="s">
         <v>52</v>

</xml_diff>

<commit_message>
Update backlog task in sprint 2
</commit_message>
<xml_diff>
--- a/QA Backlog.xlsx
+++ b/QA Backlog.xlsx
@@ -603,7 +603,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -708,11 +707,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="113147904"/>
-        <c:axId val="51496640"/>
+        <c:axId val="53256704"/>
+        <c:axId val="53085888"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="113147904"/>
+        <c:axId val="53256704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -722,7 +721,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="51496640"/>
+        <c:crossAx val="53085888"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -730,7 +729,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="51496640"/>
+        <c:axId val="53085888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -741,7 +740,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="113147904"/>
+        <c:crossAx val="53256704"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2144,8 +2143,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
update sprint 2 backlog
</commit_message>
<xml_diff>
--- a/QA Backlog.xlsx
+++ b/QA Backlog.xlsx
@@ -1,28 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\study\Capstone\Document\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="60" windowWidth="20115" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="60" windowWidth="15120" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="1" r:id="rId1"/>
     <sheet name="Sprint 1" sheetId="2" r:id="rId2"/>
     <sheet name="Sprint 2" sheetId="4" r:id="rId3"/>
-    <sheet name="Sprint 3" sheetId="3" r:id="rId4"/>
+    <sheet name="Sprint 3" sheetId="5" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="152511" concurrentCalc="0"/>
+  <calcPr calcId="144525" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="123">
   <si>
     <t>No</t>
   </si>
@@ -264,9 +259,6 @@
     <t>Total hours</t>
   </si>
   <si>
-    <t>New</t>
-  </si>
-  <si>
     <t>Total actual hours</t>
   </si>
   <si>
@@ -363,19 +355,46 @@
     <t>Fix ERD</t>
   </si>
   <si>
-    <t>Waiting for Approval</t>
-  </si>
-  <si>
     <t>Fix System architecture</t>
   </si>
   <si>
     <t>Sprint 1 task (ThiTD -&gt; MinhKH)</t>
+  </si>
+  <si>
+    <t>TungTD-&gt;MinhKH</t>
+  </si>
+  <si>
+    <t>Sprint 1 task -&gt; MinhKH</t>
+  </si>
+  <si>
+    <t>Sprint 1 task -&gt;MinhKH</t>
+  </si>
+  <si>
+    <t>26/05</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Design physical diagram </t>
+  </si>
+  <si>
+    <t>DB</t>
+  </si>
+  <si>
+    <t>Design suggest page</t>
+  </si>
+  <si>
+    <t>Design forgotton password pop-up</t>
+  </si>
+  <si>
+    <t>Fix create account form</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="dd/mm"/>
+  </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -421,7 +440,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -437,6 +456,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -481,7 +506,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -502,6 +527,10 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -606,6 +635,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -635,6 +665,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -710,11 +741,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="642379872"/>
-        <c:axId val="642380432"/>
+        <c:axId val="61546496"/>
+        <c:axId val="78071488"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="642379872"/>
+        <c:axId val="61546496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -724,7 +755,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="642380432"/>
+        <c:crossAx val="78071488"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -732,7 +763,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="642380432"/>
+        <c:axId val="78071488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -743,13 +774,498 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="642379872"/>
+        <c:crossAx val="61546496"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:dLblPos val="ctr"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="1"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Sprint 2'!$B$41:$B$42</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>Completed task</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Not completed task</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sprint 2'!$C$41:$C$42</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="ctr"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
+        </c:dLbls>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Sprint 2'!$E$45</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Performance</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Sprint 2'!$B$46:$B$49</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>MinhKH</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>KhangTN</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>TungTD</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sprint 2'!$E$46:$E$49</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="62907392"/>
+        <c:axId val="119445120"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="62907392"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="119445120"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="119445120"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="0%" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="62907392"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:dLblPos val="ctr"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="1"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Sprint 3'!$B$41:$B$42</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>Completed task</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Not completed task</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sprint 3'!$C$41:$C$42</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="ctr"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
+        </c:dLbls>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Sprint 3'!$E$45</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Performance</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Sprint 3'!$B$46:$B$49</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>MinhKH</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>KhangTN</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>TungTD</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sprint 3'!$E$46:$E$49</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="53839872"/>
+        <c:axId val="135714432"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="53839872"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="135714432"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="135714432"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="0%" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="53839872"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -829,6 +1345,144 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>133350</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>285750</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>361950</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>133350</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>285750</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>361950</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -872,7 +1526,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -907,7 +1561,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1303,7 +1957,7 @@
         <v>19</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
@@ -1314,7 +1968,7 @@
         <v>20</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
@@ -1404,8 +2058,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M46"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="B42" sqref="B42:E46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1480,7 +2134,7 @@
         <v>10</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
@@ -1502,7 +2156,7 @@
         <v>60</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D5" s="11" t="s">
         <v>74</v>
@@ -1511,7 +2165,7 @@
         <v>6</v>
       </c>
       <c r="F5" s="11" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G5" s="11"/>
       <c r="H5" s="11"/>
@@ -1529,7 +2183,7 @@
         <v>61</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D6" s="11" t="s">
         <v>74</v>
@@ -1538,7 +2192,7 @@
         <v>6</v>
       </c>
       <c r="F6" s="11" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G6" s="11"/>
       <c r="H6" s="11"/>
@@ -1553,10 +2207,10 @@
         <v>4</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D7" s="11" t="s">
         <v>74</v>
@@ -1565,7 +2219,7 @@
         <v>6</v>
       </c>
       <c r="F7" s="11" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G7" s="11"/>
       <c r="H7" s="11"/>
@@ -1583,7 +2237,7 @@
         <v>62</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D8" s="11" t="s">
         <v>75</v>
@@ -1592,7 +2246,7 @@
         <v>8</v>
       </c>
       <c r="F8" s="11" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G8" s="11"/>
       <c r="H8" s="11"/>
@@ -1610,7 +2264,7 @@
         <v>63</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D9" s="11" t="s">
         <v>75</v>
@@ -1619,7 +2273,7 @@
         <v>8</v>
       </c>
       <c r="F9" s="11" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G9" s="11"/>
       <c r="H9" s="11"/>
@@ -1637,7 +2291,7 @@
         <v>64</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D10" s="11" t="s">
         <v>75</v>
@@ -1646,7 +2300,7 @@
         <v>8</v>
       </c>
       <c r="F10" s="11" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G10" s="11"/>
       <c r="H10" s="11"/>
@@ -1664,7 +2318,7 @@
         <v>65</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>74</v>
@@ -1673,7 +2327,7 @@
         <v>4</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
@@ -1698,7 +2352,7 @@
         <v>3</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G12" s="2">
         <v>3</v>
@@ -1725,7 +2379,7 @@
         <v>8</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
@@ -1754,7 +2408,7 @@
         <v>15</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
@@ -1775,10 +2429,10 @@
         <v>12</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D15" s="11" t="s">
         <v>74</v>
@@ -1787,7 +2441,7 @@
         <v>10</v>
       </c>
       <c r="F15" s="11" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G15" s="11"/>
       <c r="H15" s="11"/>
@@ -1812,7 +2466,7 @@
         <v>12</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
@@ -1841,7 +2495,7 @@
         <v>10</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
@@ -1863,7 +2517,7 @@
         <v>71</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>75</v>
@@ -1872,7 +2526,7 @@
         <v>8</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
@@ -1897,7 +2551,7 @@
         <v>3</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
@@ -1914,7 +2568,7 @@
         <v>17</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C20" s="2"/>
       <c r="D20" s="2" t="s">
@@ -1924,7 +2578,7 @@
         <v>4</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
@@ -1987,7 +2641,7 @@
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B29" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="30" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
@@ -2024,7 +2678,7 @@
     </row>
     <row r="37" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B37" s="9" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C37" s="2">
         <f>COUNTA(F4:F20)</f>
@@ -2033,7 +2687,7 @@
     </row>
     <row r="38" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B38" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C38" s="2">
         <f>COUNTIF(F4:F20,"Completed")</f>
@@ -2042,7 +2696,7 @@
     </row>
     <row r="39" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B39" s="9" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C39" s="2">
         <f>C37-C38</f>
@@ -2054,13 +2708,13 @@
         <v>78</v>
       </c>
       <c r="C42" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="D42" s="9" t="s">
         <v>98</v>
       </c>
-      <c r="D42" s="9" t="s">
-        <v>99</v>
-      </c>
       <c r="E42" s="9" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="43" spans="2:5" x14ac:dyDescent="0.2">
@@ -2144,10 +2798,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M37"/>
+  <dimension ref="A1:M49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2164,19 +2818,19 @@
   <sheetData>
     <row r="1" spans="1:13" ht="25.5" x14ac:dyDescent="0.35">
       <c r="B1" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G1" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="I1" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>96</v>
-      </c>
-      <c r="I1" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
@@ -2225,7 +2879,7 @@
         <v>1</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="2" t="s">
@@ -2250,7 +2904,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C5" s="2"/>
       <c r="D5" s="2" t="s">
@@ -2260,7 +2914,7 @@
         <v>12</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
@@ -2275,7 +2929,7 @@
         <v>3</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C6" s="2"/>
       <c r="D6" s="2" t="s">
@@ -2285,7 +2939,7 @@
         <v>8</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>113</v>
+        <v>86</v>
       </c>
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
@@ -2295,62 +2949,66 @@
       <c r="L6" s="2"/>
       <c r="M6" s="2"/>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A7" s="2">
+    <row r="7" spans="1:13" s="17" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="16">
         <v>4</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="16" t="s">
+        <v>91</v>
+      </c>
+      <c r="C7" s="16" t="s">
+        <v>114</v>
+      </c>
+      <c r="D7" s="16" t="s">
+        <v>75</v>
+      </c>
+      <c r="E7" s="16">
+        <v>8</v>
+      </c>
+      <c r="F7" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="G7" s="16"/>
+      <c r="H7" s="16"/>
+      <c r="I7" s="16"/>
+      <c r="J7" s="16"/>
+      <c r="K7" s="16"/>
+      <c r="L7" s="16"/>
+      <c r="M7" s="16"/>
+    </row>
+    <row r="8" spans="1:13" s="17" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="16">
+        <v>5</v>
+      </c>
+      <c r="B8" s="16" t="s">
         <v>92</v>
       </c>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2" t="s">
+      <c r="C8" s="16" t="s">
+        <v>114</v>
+      </c>
+      <c r="D8" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="E7" s="2">
+      <c r="E8" s="16">
         <v>8</v>
       </c>
-      <c r="F7" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
-      <c r="I7" s="2"/>
-      <c r="J7" s="2"/>
-      <c r="K7" s="2"/>
-      <c r="L7" s="2"/>
-      <c r="M7" s="2"/>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A8" s="2">
-        <v>5</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="E8" s="2">
-        <v>8</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
-      <c r="I8" s="2"/>
-      <c r="J8" s="2"/>
-      <c r="K8" s="2"/>
-      <c r="L8" s="2"/>
-      <c r="M8" s="2"/>
+      <c r="F8" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="G8" s="16"/>
+      <c r="H8" s="16"/>
+      <c r="I8" s="16"/>
+      <c r="J8" s="16"/>
+      <c r="K8" s="16"/>
+      <c r="L8" s="16"/>
+      <c r="M8" s="16"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>6</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="2" t="s">
@@ -2360,7 +3018,7 @@
         <v>10</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>113</v>
+        <v>86</v>
       </c>
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
@@ -2375,7 +3033,7 @@
         <v>7</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C10" s="2"/>
       <c r="D10" s="2" t="s">
@@ -2385,7 +3043,7 @@
         <v>16</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>113</v>
+        <v>86</v>
       </c>
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
@@ -2403,7 +3061,7 @@
         <v>60</v>
       </c>
       <c r="C11" s="13" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D11" s="14" t="s">
         <v>52</v>
@@ -2430,7 +3088,7 @@
         <v>61</v>
       </c>
       <c r="C12" s="13" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D12" s="14" t="s">
         <v>52</v>
@@ -2449,120 +3107,120 @@
       <c r="L12" s="14"/>
       <c r="M12" s="14"/>
     </row>
-    <row r="13" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="2">
+    <row r="13" spans="1:13" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="11">
         <v>10</v>
       </c>
-      <c r="B13" s="14" t="s">
-        <v>84</v>
-      </c>
-      <c r="C13" s="13" t="s">
+      <c r="B13" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="D13" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="E13" s="11">
+        <v>6</v>
+      </c>
+      <c r="F13" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="G13" s="11"/>
+      <c r="H13" s="11"/>
+      <c r="I13" s="11"/>
+      <c r="J13" s="11"/>
+      <c r="K13" s="11"/>
+      <c r="L13" s="11"/>
+      <c r="M13" s="11"/>
+    </row>
+    <row r="14" spans="1:13" s="17" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="16">
+        <v>11</v>
+      </c>
+      <c r="B14" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="C14" s="16" t="s">
         <v>115</v>
       </c>
-      <c r="D13" s="14" t="s">
-        <v>52</v>
-      </c>
-      <c r="E13" s="14">
-        <v>6</v>
-      </c>
-      <c r="F13" s="14" t="s">
+      <c r="D14" s="16" t="s">
+        <v>75</v>
+      </c>
+      <c r="E14" s="16">
+        <v>8</v>
+      </c>
+      <c r="F14" s="16" t="s">
         <v>86</v>
       </c>
-      <c r="G13" s="14"/>
-      <c r="H13" s="14"/>
-      <c r="I13" s="14"/>
-      <c r="J13" s="14"/>
-      <c r="K13" s="14"/>
-      <c r="L13" s="14"/>
-      <c r="M13" s="14"/>
-    </row>
-    <row r="14" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="2">
-        <v>11</v>
-      </c>
-      <c r="B14" s="14" t="s">
-        <v>62</v>
-      </c>
-      <c r="C14" s="13" t="s">
-        <v>108</v>
-      </c>
-      <c r="D14" s="14" t="s">
+      <c r="G14" s="16"/>
+      <c r="H14" s="16"/>
+      <c r="I14" s="16"/>
+      <c r="J14" s="16"/>
+      <c r="K14" s="16"/>
+      <c r="L14" s="16"/>
+      <c r="M14" s="16"/>
+    </row>
+    <row r="15" spans="1:13" s="17" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="16">
+        <v>12</v>
+      </c>
+      <c r="B15" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="C15" s="16" t="s">
+        <v>116</v>
+      </c>
+      <c r="D15" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="E14" s="14">
+      <c r="E15" s="16">
         <v>8</v>
       </c>
-      <c r="F14" s="14" t="s">
+      <c r="F15" s="16" t="s">
         <v>86</v>
       </c>
-      <c r="G14" s="14"/>
-      <c r="H14" s="14"/>
-      <c r="I14" s="14"/>
-      <c r="J14" s="14"/>
-      <c r="K14" s="14"/>
-      <c r="L14" s="14"/>
-      <c r="M14" s="14"/>
-    </row>
-    <row r="15" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="2">
-        <v>12</v>
-      </c>
-      <c r="B15" s="14" t="s">
-        <v>63</v>
-      </c>
-      <c r="C15" s="13" t="s">
-        <v>108</v>
-      </c>
-      <c r="D15" s="14" t="s">
+      <c r="G15" s="16"/>
+      <c r="H15" s="16"/>
+      <c r="I15" s="16"/>
+      <c r="J15" s="16"/>
+      <c r="K15" s="16"/>
+      <c r="L15" s="16"/>
+      <c r="M15" s="16"/>
+    </row>
+    <row r="16" spans="1:13" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="11">
+        <v>13</v>
+      </c>
+      <c r="B16" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="C16" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="D16" s="11" t="s">
         <v>75</v>
       </c>
-      <c r="E15" s="14">
+      <c r="E16" s="11">
         <v>8</v>
       </c>
-      <c r="F15" s="14" t="s">
-        <v>86</v>
-      </c>
-      <c r="G15" s="14"/>
-      <c r="H15" s="14"/>
-      <c r="I15" s="14"/>
-      <c r="J15" s="14"/>
-      <c r="K15" s="14"/>
-      <c r="L15" s="14"/>
-      <c r="M15" s="14"/>
-    </row>
-    <row r="16" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="2">
-        <v>13</v>
-      </c>
-      <c r="B16" s="14" t="s">
-        <v>64</v>
-      </c>
-      <c r="C16" s="13" t="s">
-        <v>108</v>
-      </c>
-      <c r="D16" s="14" t="s">
-        <v>75</v>
-      </c>
-      <c r="E16" s="14">
-        <v>8</v>
-      </c>
-      <c r="F16" s="14" t="s">
-        <v>86</v>
-      </c>
-      <c r="G16" s="14"/>
-      <c r="H16" s="14"/>
-      <c r="I16" s="14"/>
-      <c r="J16" s="14"/>
-      <c r="K16" s="14"/>
-      <c r="L16" s="14"/>
-      <c r="M16" s="14"/>
+      <c r="F16" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="G16" s="11"/>
+      <c r="H16" s="11"/>
+      <c r="I16" s="11"/>
+      <c r="J16" s="11"/>
+      <c r="K16" s="11"/>
+      <c r="L16" s="11"/>
+      <c r="M16" s="11"/>
     </row>
     <row r="17" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
         <v>14</v>
       </c>
       <c r="B17" s="14" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C17" s="13"/>
       <c r="D17" s="14" t="s">
@@ -2572,7 +3230,7 @@
         <v>1</v>
       </c>
       <c r="F17" s="14" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G17" s="14"/>
       <c r="H17" s="14"/>
@@ -2587,7 +3245,7 @@
         <v>15</v>
       </c>
       <c r="B18" s="14" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C18" s="13"/>
       <c r="D18" s="14" t="s">
@@ -2597,7 +3255,7 @@
         <v>2</v>
       </c>
       <c r="F18" s="14" t="s">
-        <v>113</v>
+        <v>86</v>
       </c>
       <c r="G18" s="14"/>
       <c r="H18" s="14"/>
@@ -2612,7 +3270,7 @@
         <v>16</v>
       </c>
       <c r="B19" s="14" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C19" s="13"/>
       <c r="D19" s="14" t="s">
@@ -2622,7 +3280,7 @@
         <v>2</v>
       </c>
       <c r="F19" s="14" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="G19" s="14"/>
       <c r="H19" s="14"/>
@@ -2709,13 +3367,8 @@
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B29" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="C29" s="2">
-        <f>SUMIF(D4:D22,B29,E4:E22)</f>
-        <v>0</v>
-      </c>
+      <c r="B29" s="2"/>
+      <c r="C29" s="2"/>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B30" s="2" t="s">
@@ -2728,10 +3381,10 @@
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B32" s="1" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.2">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="33" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B33" s="5" t="s">
         <v>78</v>
       </c>
@@ -2739,29 +3392,122 @@
         <v>79</v>
       </c>
     </row>
-    <row r="34" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B34" s="2" t="s">
         <v>52</v>
       </c>
       <c r="C34" s="2"/>
     </row>
-    <row r="35" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B35" s="2" t="s">
         <v>73</v>
       </c>
       <c r="C35" s="2"/>
     </row>
-    <row r="36" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B36" s="2" t="s">
-        <v>74</v>
-      </c>
+    <row r="36" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B36" s="2"/>
       <c r="C36" s="2"/>
     </row>
-    <row r="37" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B37" s="2" t="s">
         <v>75</v>
       </c>
       <c r="C37" s="2"/>
+    </row>
+    <row r="40" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B40" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="C40" s="2">
+        <f>COUNTA(F4:F19)</f>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="41" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B41" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="C41" s="2">
+        <f>COUNTIF(F4:F19,"Completed")</f>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="42" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B42" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="C42" s="2">
+        <f>C40-C41</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="45" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B45" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="C45" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="D45" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="E45" s="9" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="46" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B46" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C46" s="2">
+        <f>COUNTIF(D4:D19,B46)</f>
+        <v>6</v>
+      </c>
+      <c r="D46" s="2">
+        <v>9</v>
+      </c>
+      <c r="E46" s="10">
+        <f>D46/C46</f>
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="47" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B47" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C47" s="2">
+        <f>COUNTIF(D4:D19,B47)</f>
+        <v>5</v>
+      </c>
+      <c r="D47" s="2">
+        <v>5</v>
+      </c>
+      <c r="E47" s="10">
+        <f t="shared" ref="E47:E49" si="0">D47/C47</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B48" s="2"/>
+      <c r="C48" s="2"/>
+      <c r="D48" s="2"/>
+      <c r="E48" s="10"/>
+    </row>
+    <row r="49" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B49" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C49" s="2">
+        <f>COUNTIF(D4:D19,B49)</f>
+        <v>5</v>
+      </c>
+      <c r="D49" s="2">
+        <v>0</v>
+      </c>
+      <c r="E49" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <dataValidations count="2">
@@ -2774,19 +3520,606 @@
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:M49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="1"/>
+    <col min="2" max="2" width="36.42578125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="17.85546875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="14.42578125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="18" style="1" customWidth="1"/>
+    <col min="6" max="6" width="21.7109375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="9.140625" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" ht="25.5" x14ac:dyDescent="0.35">
+      <c r="B1" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="H1" s="19" t="s">
+        <v>117</v>
+      </c>
+      <c r="I1" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="J1" s="19">
+        <v>42041</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A3" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="J3" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="K3" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="L3" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="M3" s="5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A4" s="2">
+        <v>1</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
+      <c r="L4" s="2"/>
+      <c r="M4" s="2"/>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A5" s="2">
+        <v>2</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
+      <c r="L5" s="2"/>
+      <c r="M5" s="2"/>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A6" s="2">
+        <v>3</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
+      <c r="L6" s="2"/>
+      <c r="M6" s="2"/>
+    </row>
+    <row r="7" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="2">
+        <v>4</v>
+      </c>
+      <c r="B7" s="14" t="s">
+        <v>122</v>
+      </c>
+      <c r="C7" s="14"/>
+      <c r="D7" s="14"/>
+      <c r="E7" s="14"/>
+      <c r="F7" s="14"/>
+      <c r="G7" s="14"/>
+      <c r="H7" s="14"/>
+      <c r="I7" s="14"/>
+      <c r="J7" s="14"/>
+      <c r="K7" s="14"/>
+      <c r="L7" s="14"/>
+      <c r="M7" s="14"/>
+    </row>
+    <row r="8" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="2">
+        <v>5</v>
+      </c>
+      <c r="B8" s="14"/>
+      <c r="C8" s="14"/>
+      <c r="D8" s="14"/>
+      <c r="E8" s="14"/>
+      <c r="F8" s="14"/>
+      <c r="G8" s="14"/>
+      <c r="H8" s="14"/>
+      <c r="I8" s="14"/>
+      <c r="J8" s="14"/>
+      <c r="K8" s="14"/>
+      <c r="L8" s="14"/>
+      <c r="M8" s="14"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A9" s="2">
+        <v>6</v>
+      </c>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="2"/>
+      <c r="L9" s="2"/>
+      <c r="M9" s="2"/>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A10" s="2">
+        <v>7</v>
+      </c>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
+      <c r="J10" s="2"/>
+      <c r="K10" s="2"/>
+      <c r="L10" s="2"/>
+      <c r="M10" s="2"/>
+    </row>
+    <row r="11" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="2">
+        <v>8</v>
+      </c>
+      <c r="B11" s="14"/>
+      <c r="C11" s="13"/>
+      <c r="D11" s="14"/>
+      <c r="E11" s="14"/>
+      <c r="F11" s="14"/>
+      <c r="G11" s="14"/>
+      <c r="H11" s="14"/>
+      <c r="I11" s="14"/>
+      <c r="J11" s="14"/>
+      <c r="K11" s="14"/>
+      <c r="L11" s="14"/>
+      <c r="M11" s="14"/>
+    </row>
+    <row r="12" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="2">
+        <v>9</v>
+      </c>
+      <c r="B12" s="14"/>
+      <c r="C12" s="13"/>
+      <c r="D12" s="14"/>
+      <c r="E12" s="14"/>
+      <c r="F12" s="14"/>
+      <c r="G12" s="14"/>
+      <c r="H12" s="14"/>
+      <c r="I12" s="14"/>
+      <c r="J12" s="14"/>
+      <c r="K12" s="14"/>
+      <c r="L12" s="14"/>
+      <c r="M12" s="14"/>
+    </row>
+    <row r="13" spans="1:13" s="18" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="2">
+        <v>10</v>
+      </c>
+      <c r="B13" s="13"/>
+      <c r="C13" s="13"/>
+      <c r="D13" s="13"/>
+      <c r="E13" s="13"/>
+      <c r="F13" s="13"/>
+      <c r="G13" s="13"/>
+      <c r="H13" s="13"/>
+      <c r="I13" s="13"/>
+      <c r="J13" s="13"/>
+      <c r="K13" s="13"/>
+      <c r="L13" s="13"/>
+      <c r="M13" s="13"/>
+    </row>
+    <row r="14" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="2">
+        <v>11</v>
+      </c>
+      <c r="B14" s="14"/>
+      <c r="C14" s="14"/>
+      <c r="D14" s="14"/>
+      <c r="E14" s="14"/>
+      <c r="F14" s="14"/>
+      <c r="G14" s="14"/>
+      <c r="H14" s="14"/>
+      <c r="I14" s="14"/>
+      <c r="J14" s="14"/>
+      <c r="K14" s="14"/>
+      <c r="L14" s="14"/>
+      <c r="M14" s="14"/>
+    </row>
+    <row r="15" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="2">
+        <v>12</v>
+      </c>
+      <c r="B15" s="14"/>
+      <c r="C15" s="14"/>
+      <c r="D15" s="14"/>
+      <c r="E15" s="14"/>
+      <c r="F15" s="14"/>
+      <c r="G15" s="14"/>
+      <c r="H15" s="14"/>
+      <c r="I15" s="14"/>
+      <c r="J15" s="14"/>
+      <c r="K15" s="14"/>
+      <c r="L15" s="14"/>
+      <c r="M15" s="14"/>
+    </row>
+    <row r="16" spans="1:13" s="18" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="2">
+        <v>13</v>
+      </c>
+      <c r="B16" s="13"/>
+      <c r="C16" s="13"/>
+      <c r="D16" s="13"/>
+      <c r="E16" s="13"/>
+      <c r="F16" s="13"/>
+      <c r="G16" s="13"/>
+      <c r="H16" s="13"/>
+      <c r="I16" s="13"/>
+      <c r="J16" s="13"/>
+      <c r="K16" s="13"/>
+      <c r="L16" s="13"/>
+      <c r="M16" s="13"/>
+    </row>
+    <row r="17" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="2">
+        <v>14</v>
+      </c>
+      <c r="B17" s="14"/>
+      <c r="C17" s="13"/>
+      <c r="D17" s="14"/>
+      <c r="E17" s="14"/>
+      <c r="F17" s="14"/>
+      <c r="G17" s="14"/>
+      <c r="H17" s="14"/>
+      <c r="I17" s="14"/>
+      <c r="J17" s="14"/>
+      <c r="K17" s="14"/>
+      <c r="L17" s="14"/>
+      <c r="M17" s="14"/>
+    </row>
+    <row r="18" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="2">
+        <v>15</v>
+      </c>
+      <c r="B18" s="14"/>
+      <c r="C18" s="13"/>
+      <c r="D18" s="14"/>
+      <c r="E18" s="14"/>
+      <c r="F18" s="14"/>
+      <c r="G18" s="14"/>
+      <c r="H18" s="14"/>
+      <c r="I18" s="14"/>
+      <c r="J18" s="14"/>
+      <c r="K18" s="14"/>
+      <c r="L18" s="14"/>
+      <c r="M18" s="14"/>
+    </row>
+    <row r="19" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="2">
+        <v>16</v>
+      </c>
+      <c r="B19" s="14"/>
+      <c r="C19" s="13"/>
+      <c r="D19" s="14"/>
+      <c r="E19" s="14"/>
+      <c r="F19" s="14"/>
+      <c r="G19" s="14"/>
+      <c r="H19" s="14"/>
+      <c r="I19" s="14"/>
+      <c r="J19" s="14"/>
+      <c r="K19" s="14"/>
+      <c r="L19" s="14"/>
+      <c r="M19" s="14"/>
+    </row>
+    <row r="20" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="2">
+        <v>17</v>
+      </c>
+      <c r="B20" s="14"/>
+      <c r="C20" s="13"/>
+      <c r="D20" s="14"/>
+      <c r="E20" s="14"/>
+      <c r="F20" s="14"/>
+      <c r="G20" s="14"/>
+      <c r="H20" s="14"/>
+      <c r="I20" s="14"/>
+      <c r="J20" s="14"/>
+      <c r="K20" s="14"/>
+      <c r="L20" s="14"/>
+      <c r="M20" s="14"/>
+    </row>
+    <row r="21" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="2">
+        <v>18</v>
+      </c>
+      <c r="B21" s="14"/>
+      <c r="C21" s="13"/>
+      <c r="D21" s="14"/>
+      <c r="E21" s="14"/>
+      <c r="F21" s="14"/>
+      <c r="G21" s="14"/>
+      <c r="H21" s="14"/>
+      <c r="I21" s="14"/>
+      <c r="J21" s="14"/>
+      <c r="K21" s="14"/>
+      <c r="L21" s="14"/>
+      <c r="M21" s="14"/>
+    </row>
+    <row r="22" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="2">
+        <v>19</v>
+      </c>
+      <c r="B22" s="14"/>
+      <c r="C22" s="13"/>
+      <c r="D22" s="14"/>
+      <c r="E22" s="14"/>
+      <c r="F22" s="14"/>
+      <c r="G22" s="14"/>
+      <c r="H22" s="14"/>
+      <c r="I22" s="14"/>
+      <c r="J22" s="14"/>
+      <c r="K22" s="14"/>
+      <c r="L22" s="14"/>
+      <c r="M22" s="14"/>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B25" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B26" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B27" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C27" s="2">
+        <f>SUMIF(D4:D22,B27,E4:E22)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B28" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C28" s="2">
+        <f>SUMIF(D4:D22,B28,E4:E22)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B29" s="2"/>
+      <c r="C29" s="2"/>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B30" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C30" s="2">
+        <f>SUMIF(D4:D22,B30,E4:E22)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B32" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="33" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B33" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="34" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B34" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C34" s="2"/>
+    </row>
+    <row r="35" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B35" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C35" s="2"/>
+    </row>
+    <row r="36" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B36" s="2"/>
+      <c r="C36" s="2"/>
+    </row>
+    <row r="37" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B37" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C37" s="2"/>
+    </row>
+    <row r="40" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B40" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="C40" s="2">
+        <f>COUNTA(F4:F19)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B41" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="C41" s="2">
+        <f>COUNTIF(F4:F19,"Completed")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B42" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="C42" s="2">
+        <f>C40-C41</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B45" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="C45" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="D45" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="E45" s="9" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="46" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B46" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C46" s="2">
+        <f>COUNTIF(D4:D19,B46)</f>
+        <v>0</v>
+      </c>
+      <c r="D46" s="2">
+        <v>9</v>
+      </c>
+      <c r="E46" s="10" t="e">
+        <f>D46/C46</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="47" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B47" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C47" s="2">
+        <f>COUNTIF(D4:D19,B47)</f>
+        <v>0</v>
+      </c>
+      <c r="D47" s="2">
+        <v>5</v>
+      </c>
+      <c r="E47" s="10" t="e">
+        <f t="shared" ref="E47:E49" si="0">D47/C47</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="48" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B48" s="2"/>
+      <c r="C48" s="2"/>
+      <c r="D48" s="2"/>
+      <c r="E48" s="10"/>
+    </row>
+    <row r="49" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B49" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C49" s="2">
+        <f>COUNTIF(D4:D19,B49)</f>
+        <v>0</v>
+      </c>
+      <c r="D49" s="2">
+        <v>0</v>
+      </c>
+      <c r="E49" s="10" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D4:D22">
+      <formula1>"MinhKH, KhangTN, ThiTD, TungTD"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F4:F22">
+      <formula1>"New, In process, Waiting for Approval, Completed"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update status sprint 3, create sprint 4
</commit_message>
<xml_diff>
--- a/QA Backlog.xlsx
+++ b/QA Backlog.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TaDucTung\University\Document\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="240" yWindow="60" windowWidth="15120" windowHeight="8010" activeTab="3"/>
   </bookViews>
@@ -16,13 +11,14 @@
     <sheet name="Sprint 1" sheetId="2" r:id="rId2"/>
     <sheet name="Sprint 2" sheetId="4" r:id="rId3"/>
     <sheet name="Sprint 3" sheetId="5" r:id="rId4"/>
+    <sheet name="Sprint 4" sheetId="6" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="152511" concurrentCalc="0"/>
+  <calcPr calcId="144525" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="152">
   <si>
     <t>No</t>
   </si>
@@ -402,21 +398,6 @@
     <t>Create dao, dto</t>
   </si>
   <si>
-    <t>demo real-time notification</t>
-  </si>
-  <si>
-    <t>code login function</t>
-  </si>
-  <si>
-    <t>code register function</t>
-  </si>
-  <si>
-    <t>code newsfeed page</t>
-  </si>
-  <si>
-    <t>Design manage material</t>
-  </si>
-  <si>
     <t>New</t>
   </si>
   <si>
@@ -427,6 +408,72 @@
   </si>
   <si>
     <t>Waiting for Approval</t>
+  </si>
+  <si>
+    <t>include client side validation</t>
+  </si>
+  <si>
+    <t>real-time notification &amp; discussion demo</t>
+  </si>
+  <si>
+    <t>notification count, left notification, real-time disscussion</t>
+  </si>
+  <si>
+    <t>Sprint 4</t>
+  </si>
+  <si>
+    <t>implement login function</t>
+  </si>
+  <si>
+    <t>implement register function</t>
+  </si>
+  <si>
+    <t>implement newsfeed page</t>
+  </si>
+  <si>
+    <t>Implement search function</t>
+  </si>
+  <si>
+    <t>Implement upload and manage material</t>
+  </si>
+  <si>
+    <t>Implement follow/unfollow teacher function</t>
+  </si>
+  <si>
+    <t>Implement request function</t>
+  </si>
+  <si>
+    <t>Implement invitation function</t>
+  </si>
+  <si>
+    <t>Implement create class function</t>
+  </si>
+  <si>
+    <t>Implement create post function</t>
+  </si>
+  <si>
+    <t>include article, question and material</t>
+  </si>
+  <si>
+    <t>store material using blob demo</t>
+  </si>
+  <si>
+    <t>Implement edit profile function</t>
+  </si>
+  <si>
+    <t>Implement suggest related post function</t>
+  </si>
+  <si>
+    <t>teacher profile, student profile</t>
+  </si>
+  <si>
+    <t>solr</t>
+  </si>
+  <si>
+    <t>Design Manage material UI</t>
+  </si>
+  <si>
+    <t>Design Manage Material UI</t>
   </si>
 </sst>
 </file>
@@ -547,7 +594,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -573,6 +620,8 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -677,6 +726,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -706,6 +756,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -781,11 +832,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="224652752"/>
-        <c:axId val="224653312"/>
+        <c:axId val="54149120"/>
+        <c:axId val="76039872"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="224652752"/>
+        <c:axId val="54149120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -795,7 +846,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="224653312"/>
+        <c:crossAx val="76039872"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -803,7 +854,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="224653312"/>
+        <c:axId val="76039872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -814,13 +865,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="224652752"/>
+        <c:crossAx val="54149120"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -922,6 +974,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -951,6 +1004,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1020,11 +1074,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="224657232"/>
-        <c:axId val="224657792"/>
+        <c:axId val="54151168"/>
+        <c:axId val="76042752"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="224657232"/>
+        <c:axId val="54151168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1034,7 +1088,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="224657792"/>
+        <c:crossAx val="76042752"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1042,7 +1096,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="224657792"/>
+        <c:axId val="76042752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1053,13 +1107,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="224657232"/>
+        <c:crossAx val="54151168"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1139,10 +1194,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>11</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1242,10 +1297,10 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>2.25</c:v>
+                  <c:v>0.83333333333333337</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.6666666666666667</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
@@ -1263,11 +1318,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="50014064"/>
-        <c:axId val="50012944"/>
+        <c:axId val="59510784"/>
+        <c:axId val="76045632"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="50014064"/>
+        <c:axId val="59510784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1277,7 +1332,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="50012944"/>
+        <c:crossAx val="76045632"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1285,7 +1340,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="50012944"/>
+        <c:axId val="76045632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1296,7 +1351,251 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="50014064"/>
+        <c:crossAx val="59510784"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:dLblPos val="ctr"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="1"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Sprint 4'!$B$41:$B$42</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>Completed task</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Not completed task</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sprint 4'!$C$41:$C$42</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="ctr"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
+        </c:dLbls>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Sprint 4'!$E$45</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Performance</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Sprint 4'!$B$46:$B$49</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>MinhKH</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>KhangTN</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>TungTD</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sprint 4'!$E$46:$E$49</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1.6666666666666667</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="98111488"/>
+        <c:axId val="97951744"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="98111488"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="97951744"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="97951744"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="0%" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="98111488"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1521,6 +1820,75 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>133350</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>285750</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>361950</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -1564,7 +1932,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1599,7 +1967,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1811,7 +2179,7 @@
   <dimension ref="A1:C24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1833,25 +2201,25 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="2">
+    <row r="2" spans="1:3" s="22" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="21">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="21" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" s="2">
+    <row r="3" spans="1:3" s="22" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="21">
         <v>2</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="21" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1866,36 +2234,36 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" s="2">
+    <row r="5" spans="1:3" s="22" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="21">
         <v>4</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="21" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" s="2">
+    <row r="6" spans="1:3" s="22" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="21">
         <v>5</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="21" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" s="2">
+    <row r="7" spans="1:3" s="22" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="21">
         <v>6</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" s="21" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1910,47 +2278,47 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" s="2">
+    <row r="9" spans="1:3" s="22" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="21">
         <v>8</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C9" s="21" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" s="2">
+    <row r="10" spans="1:3" s="22" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="21">
         <v>9</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C10" s="21" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" s="2">
+    <row r="11" spans="1:3" s="22" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="21">
         <v>10</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C11" s="21" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12" s="2">
+    <row r="12" spans="1:3" s="22" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="21">
         <v>11</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="C12" s="21" t="s">
         <v>37</v>
       </c>
     </row>
@@ -3569,7 +3937,7 @@
   <dimension ref="A1:M49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3598,7 +3966,7 @@
         <v>94</v>
       </c>
       <c r="J1" s="19">
-        <v>42041</v>
+        <v>42157</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
@@ -3659,10 +4027,14 @@
         <v>8</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
+        <v>86</v>
+      </c>
+      <c r="G4" s="2">
+        <v>4</v>
+      </c>
+      <c r="H4" s="2">
+        <v>0</v>
+      </c>
       <c r="I4" s="2"/>
       <c r="J4" s="2"/>
       <c r="K4" s="2"/>
@@ -3681,42 +4053,48 @@
         <v>52</v>
       </c>
       <c r="E5" s="2">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>131</v>
+        <v>86</v>
       </c>
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
       <c r="K5" s="2"/>
-      <c r="L5" s="2"/>
-      <c r="M5" s="2"/>
+      <c r="L5" s="2">
+        <v>4</v>
+      </c>
+      <c r="M5" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>3</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>75</v>
+        <v>52</v>
       </c>
       <c r="E6" s="2">
         <v>2</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>131</v>
+        <v>86</v>
       </c>
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
-      <c r="J6" s="2"/>
+      <c r="J6" s="2">
+        <v>0</v>
+      </c>
       <c r="K6" s="2"/>
       <c r="L6" s="2"/>
       <c r="M6" s="2"/>
@@ -3725,45 +4103,49 @@
       <c r="A7" s="2">
         <v>4</v>
       </c>
-      <c r="B7" s="14" t="s">
-        <v>130</v>
-      </c>
-      <c r="C7" s="14"/>
+      <c r="B7" s="15" t="s">
+        <v>122</v>
+      </c>
+      <c r="C7" s="14" t="s">
+        <v>123</v>
+      </c>
       <c r="D7" s="14" t="s">
-        <v>73</v>
+        <v>52</v>
       </c>
       <c r="E7" s="14">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>131</v>
+        <v>86</v>
       </c>
       <c r="G7" s="14"/>
       <c r="H7" s="14"/>
       <c r="I7" s="14"/>
       <c r="J7" s="14"/>
-      <c r="K7" s="14"/>
-      <c r="L7" s="14"/>
+      <c r="K7" s="14">
+        <v>3</v>
+      </c>
+      <c r="L7" s="14">
+        <v>0</v>
+      </c>
       <c r="M7" s="14"/>
     </row>
     <row r="8" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>5</v>
       </c>
-      <c r="B8" s="15" t="s">
-        <v>122</v>
-      </c>
-      <c r="C8" s="14" t="s">
-        <v>123</v>
-      </c>
-      <c r="D8" s="14" t="s">
-        <v>52</v>
-      </c>
-      <c r="E8" s="14">
-        <v>6</v>
+      <c r="B8" s="14" t="s">
+        <v>124</v>
+      </c>
+      <c r="C8" s="14"/>
+      <c r="D8" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="E8" s="2">
+        <v>12</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>131</v>
+        <v>86</v>
       </c>
       <c r="G8" s="14"/>
       <c r="H8" s="14"/>
@@ -3777,23 +4159,27 @@
       <c r="A9" s="2">
         <v>6</v>
       </c>
-      <c r="B9" s="14" t="s">
-        <v>124</v>
-      </c>
-      <c r="C9" s="14"/>
+      <c r="B9" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="C9" s="2"/>
       <c r="D9" s="2" t="s">
-        <v>73</v>
+        <v>52</v>
       </c>
       <c r="E9" s="2">
         <v>8</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>134</v>
+        <v>86</v>
       </c>
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
-      <c r="I9" s="2"/>
-      <c r="J9" s="2"/>
+      <c r="I9" s="2">
+        <v>4</v>
+      </c>
+      <c r="J9" s="2">
+        <v>0</v>
+      </c>
       <c r="K9" s="2"/>
       <c r="L9" s="2"/>
       <c r="M9" s="2"/>
@@ -3803,17 +4189,19 @@
         <v>7</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="E10" s="2">
-        <v>8</v>
+        <v>134</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="D10" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="E10" s="14">
+        <v>10</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
@@ -3827,10 +4215,12 @@
       <c r="A11" s="2">
         <v>8</v>
       </c>
-      <c r="B11" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="C11" s="2"/>
+      <c r="B11" s="14" t="s">
+        <v>135</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>130</v>
+      </c>
       <c r="D11" s="14" t="s">
         <v>75</v>
       </c>
@@ -3838,7 +4228,7 @@
         <v>10</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="G11" s="14"/>
       <c r="H11" s="14"/>
@@ -3853,17 +4243,17 @@
         <v>9</v>
       </c>
       <c r="B12" s="14" t="s">
-        <v>128</v>
+        <v>136</v>
       </c>
       <c r="C12" s="13"/>
       <c r="D12" s="14" t="s">
         <v>75</v>
       </c>
       <c r="E12" s="14">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="G12" s="14"/>
       <c r="H12" s="14"/>
@@ -3878,17 +4268,19 @@
         <v>10</v>
       </c>
       <c r="B13" s="14" t="s">
-        <v>129</v>
-      </c>
-      <c r="C13" s="13"/>
+        <v>131</v>
+      </c>
+      <c r="C13" s="14" t="s">
+        <v>132</v>
+      </c>
       <c r="D13" s="14" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E13" s="14">
         <v>12</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>134</v>
+        <v>86</v>
       </c>
       <c r="G13" s="14"/>
       <c r="H13" s="14"/>
@@ -3903,17 +4295,17 @@
         <v>11</v>
       </c>
       <c r="B14" s="14" t="s">
-        <v>126</v>
+        <v>145</v>
       </c>
       <c r="C14" s="14"/>
       <c r="D14" s="14" t="s">
         <v>73</v>
       </c>
       <c r="E14" s="14">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>134</v>
+        <v>86</v>
       </c>
       <c r="G14" s="14"/>
       <c r="H14" s="14"/>
@@ -3924,21 +4316,31 @@
       <c r="M14" s="14"/>
     </row>
     <row r="15" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="2">
+      <c r="A15" s="20">
         <v>12</v>
       </c>
-      <c r="B15" s="13"/>
-      <c r="C15" s="13"/>
-      <c r="D15" s="13"/>
-      <c r="E15" s="13"/>
-      <c r="F15" s="13"/>
+      <c r="B15" s="14" t="s">
+        <v>150</v>
+      </c>
+      <c r="C15" s="14"/>
+      <c r="D15" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="E15" s="14">
+        <v>8</v>
+      </c>
+      <c r="F15" s="14" t="s">
+        <v>85</v>
+      </c>
       <c r="G15" s="14"/>
       <c r="H15" s="14"/>
       <c r="I15" s="14"/>
       <c r="J15" s="14"/>
       <c r="K15" s="14"/>
       <c r="L15" s="14"/>
-      <c r="M15" s="14"/>
+      <c r="M15" s="14">
+        <v>4</v>
+      </c>
     </row>
     <row r="16" spans="1:13" s="18" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
@@ -4078,7 +4480,7 @@
       </c>
       <c r="C27" s="2">
         <f>SUMIF(D4:D22,B27,E4:E22)</f>
-        <v>30</v>
+        <v>36</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.2">
@@ -4100,7 +4502,7 @@
       </c>
       <c r="C30" s="2">
         <f>SUMIF(D4:D22,B30,E4:E22)</f>
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.2">
@@ -4144,7 +4546,7 @@
       </c>
       <c r="C40" s="2">
         <f>COUNTA(F4:F19)</f>
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="41" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -4153,7 +4555,7 @@
       </c>
       <c r="C41" s="2">
         <f>COUNTIF(F4:F19,"Completed")</f>
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="42" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -4162,7 +4564,7 @@
       </c>
       <c r="C42" s="2">
         <f>C40-C41</f>
-        <v>11</v>
+        <v>4</v>
       </c>
     </row>
     <row r="45" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -4185,14 +4587,14 @@
       </c>
       <c r="C46" s="2">
         <f>COUNTIF(D4:D19,B46)</f>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D46" s="2">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="E46" s="10">
         <f>D46/C46</f>
-        <v>2.25</v>
+        <v>0.83333333333333337</v>
       </c>
     </row>
     <row r="47" spans="2:5" x14ac:dyDescent="0.2">
@@ -4204,11 +4606,11 @@
         <v>3</v>
       </c>
       <c r="D47" s="2">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E47" s="10">
         <f t="shared" ref="E47:E49" si="0">D47/C47</f>
-        <v>1.6666666666666667</v>
+        <v>1</v>
       </c>
     </row>
     <row r="48" spans="2:5" x14ac:dyDescent="0.2">
@@ -4223,7 +4625,7 @@
       </c>
       <c r="C49" s="2">
         <f>COUNTIF(D4:D19,B49)</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D49" s="2">
         <v>0</v>
@@ -4246,4 +4648,686 @@
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M49"/>
+  <sheetViews>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="1"/>
+    <col min="2" max="2" width="36.42578125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="17.85546875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="14.42578125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="18" style="1" customWidth="1"/>
+    <col min="6" max="6" width="21.7109375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="9.140625" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" ht="25.5" x14ac:dyDescent="0.35">
+      <c r="B1" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="H1" s="19">
+        <v>42158</v>
+      </c>
+      <c r="I1" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="J1" s="19">
+        <v>42164</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A3" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="J3" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="K3" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="L3" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="M3" s="5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A4" s="2">
+        <v>1</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E4" s="2">
+        <v>16</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
+      <c r="L4" s="2"/>
+      <c r="M4" s="2"/>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A5" s="2">
+        <v>2</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="E5" s="2">
+        <v>16</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
+      <c r="L5" s="2"/>
+      <c r="M5" s="2"/>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A6" s="2">
+        <v>3</v>
+      </c>
+      <c r="B6" s="14" t="s">
+        <v>139</v>
+      </c>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="E6" s="2">
+        <v>6</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
+      <c r="L6" s="2"/>
+      <c r="M6" s="2"/>
+    </row>
+    <row r="7" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="2">
+        <v>4</v>
+      </c>
+      <c r="B7" s="15" t="s">
+        <v>140</v>
+      </c>
+      <c r="C7" s="14"/>
+      <c r="D7" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="E7" s="14">
+        <v>6</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="G7" s="14"/>
+      <c r="H7" s="14"/>
+      <c r="I7" s="14"/>
+      <c r="J7" s="14"/>
+      <c r="K7" s="14"/>
+      <c r="L7" s="14"/>
+      <c r="M7" s="14"/>
+    </row>
+    <row r="8" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="2">
+        <v>5</v>
+      </c>
+      <c r="B8" s="14" t="s">
+        <v>141</v>
+      </c>
+      <c r="C8" s="14"/>
+      <c r="D8" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="E8" s="2">
+        <v>6</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="G8" s="14"/>
+      <c r="H8" s="14"/>
+      <c r="I8" s="14"/>
+      <c r="J8" s="14"/>
+      <c r="K8" s="14"/>
+      <c r="L8" s="14"/>
+      <c r="M8" s="14"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A9" s="2">
+        <v>6</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="E9" s="2">
+        <v>6</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="2"/>
+      <c r="L9" s="2"/>
+      <c r="M9" s="2"/>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A10" s="2">
+        <v>7</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="D10" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="E10" s="14">
+        <v>16</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
+      <c r="J10" s="2"/>
+      <c r="K10" s="2"/>
+      <c r="L10" s="2"/>
+      <c r="M10" s="2"/>
+    </row>
+    <row r="11" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="2">
+        <v>8</v>
+      </c>
+      <c r="B11" s="14" t="s">
+        <v>146</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="D11" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="E11" s="14">
+        <v>8</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="G11" s="14"/>
+      <c r="H11" s="14"/>
+      <c r="I11" s="14"/>
+      <c r="J11" s="14"/>
+      <c r="K11" s="14"/>
+      <c r="L11" s="14"/>
+      <c r="M11" s="14"/>
+    </row>
+    <row r="12" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="2">
+        <v>9</v>
+      </c>
+      <c r="B12" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="C12" s="13"/>
+      <c r="D12" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="E12" s="14">
+        <v>12</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="G12" s="14"/>
+      <c r="H12" s="14"/>
+      <c r="I12" s="14"/>
+      <c r="J12" s="14"/>
+      <c r="K12" s="14"/>
+      <c r="L12" s="14"/>
+      <c r="M12" s="14"/>
+    </row>
+    <row r="13" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="20">
+        <v>10</v>
+      </c>
+      <c r="B13" s="14" t="s">
+        <v>151</v>
+      </c>
+      <c r="C13" s="14"/>
+      <c r="D13" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="E13" s="14">
+        <v>4</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="G13" s="14"/>
+      <c r="H13" s="14"/>
+      <c r="I13" s="14"/>
+      <c r="J13" s="14"/>
+      <c r="K13" s="14"/>
+      <c r="L13" s="14"/>
+      <c r="M13" s="14"/>
+    </row>
+    <row r="14" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="2">
+        <v>11</v>
+      </c>
+      <c r="B14" s="14"/>
+      <c r="C14" s="14"/>
+      <c r="D14" s="14"/>
+      <c r="E14" s="14"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="14"/>
+      <c r="H14" s="14"/>
+      <c r="I14" s="14"/>
+      <c r="J14" s="14"/>
+      <c r="K14" s="14"/>
+      <c r="L14" s="14"/>
+      <c r="M14" s="14"/>
+    </row>
+    <row r="15" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="2">
+        <v>12</v>
+      </c>
+      <c r="B15" s="13"/>
+      <c r="C15" s="13"/>
+      <c r="D15" s="13"/>
+      <c r="E15" s="13"/>
+      <c r="F15" s="13"/>
+      <c r="G15" s="14"/>
+      <c r="H15" s="14"/>
+      <c r="I15" s="14"/>
+      <c r="J15" s="14"/>
+      <c r="K15" s="14"/>
+      <c r="L15" s="14"/>
+      <c r="M15" s="14"/>
+    </row>
+    <row r="16" spans="1:13" s="18" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="2">
+        <v>13</v>
+      </c>
+      <c r="B16" s="13"/>
+      <c r="C16" s="13"/>
+      <c r="D16" s="13"/>
+      <c r="E16" s="13"/>
+      <c r="F16" s="13"/>
+      <c r="G16" s="13"/>
+      <c r="H16" s="13"/>
+      <c r="I16" s="13"/>
+      <c r="J16" s="13"/>
+      <c r="K16" s="13"/>
+      <c r="L16" s="13"/>
+      <c r="M16" s="13"/>
+    </row>
+    <row r="17" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="2">
+        <v>14</v>
+      </c>
+      <c r="B17" s="14"/>
+      <c r="C17" s="13"/>
+      <c r="D17" s="14"/>
+      <c r="E17" s="14"/>
+      <c r="F17" s="14"/>
+      <c r="G17" s="14"/>
+      <c r="H17" s="14"/>
+      <c r="I17" s="14"/>
+      <c r="J17" s="14"/>
+      <c r="K17" s="14"/>
+      <c r="L17" s="14"/>
+      <c r="M17" s="14"/>
+    </row>
+    <row r="18" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="2">
+        <v>15</v>
+      </c>
+      <c r="B18" s="14"/>
+      <c r="C18" s="13"/>
+      <c r="D18" s="14"/>
+      <c r="E18" s="14"/>
+      <c r="F18" s="14"/>
+      <c r="G18" s="14"/>
+      <c r="H18" s="14"/>
+      <c r="I18" s="14"/>
+      <c r="J18" s="14"/>
+      <c r="K18" s="14"/>
+      <c r="L18" s="14"/>
+      <c r="M18" s="14"/>
+    </row>
+    <row r="19" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="2">
+        <v>16</v>
+      </c>
+      <c r="B19" s="14"/>
+      <c r="C19" s="13"/>
+      <c r="D19" s="14"/>
+      <c r="E19" s="14"/>
+      <c r="F19" s="14"/>
+      <c r="G19" s="14"/>
+      <c r="H19" s="14"/>
+      <c r="I19" s="14"/>
+      <c r="J19" s="14"/>
+      <c r="K19" s="14"/>
+      <c r="L19" s="14"/>
+      <c r="M19" s="14"/>
+    </row>
+    <row r="20" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="2">
+        <v>17</v>
+      </c>
+      <c r="B20" s="14"/>
+      <c r="C20" s="13"/>
+      <c r="D20" s="14"/>
+      <c r="E20" s="14"/>
+      <c r="F20" s="14"/>
+      <c r="G20" s="14"/>
+      <c r="H20" s="14"/>
+      <c r="I20" s="14"/>
+      <c r="J20" s="14"/>
+      <c r="K20" s="14"/>
+      <c r="L20" s="14"/>
+      <c r="M20" s="14"/>
+    </row>
+    <row r="21" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="2">
+        <v>18</v>
+      </c>
+      <c r="B21" s="14"/>
+      <c r="C21" s="13"/>
+      <c r="D21" s="14"/>
+      <c r="E21" s="14"/>
+      <c r="F21" s="14"/>
+      <c r="G21" s="14"/>
+      <c r="H21" s="14"/>
+      <c r="I21" s="14"/>
+      <c r="J21" s="14"/>
+      <c r="K21" s="14"/>
+      <c r="L21" s="14"/>
+      <c r="M21" s="14"/>
+    </row>
+    <row r="22" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="2">
+        <v>19</v>
+      </c>
+      <c r="B22" s="14"/>
+      <c r="C22" s="13"/>
+      <c r="D22" s="14"/>
+      <c r="E22" s="14"/>
+      <c r="F22" s="14"/>
+      <c r="G22" s="14"/>
+      <c r="H22" s="14"/>
+      <c r="I22" s="14"/>
+      <c r="J22" s="14"/>
+      <c r="K22" s="14"/>
+      <c r="L22" s="14"/>
+      <c r="M22" s="14"/>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="E23" s="1">
+        <f>SUM(E4:E22)</f>
+        <v>96</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B25" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B26" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B27" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C27" s="2">
+        <f>SUMIF(D4:D22,B27,E4:E22)</f>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B28" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C28" s="2">
+        <f>SUMIF(D4:D22,B28,E4:E22)</f>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B29" s="2"/>
+      <c r="C29" s="2"/>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B30" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C30" s="2">
+        <f>SUMIF(D4:D22,B30,E4:E22)</f>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B32" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="33" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B33" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="34" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B34" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C34" s="2"/>
+    </row>
+    <row r="35" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B35" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C35" s="2"/>
+    </row>
+    <row r="36" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B36" s="2"/>
+      <c r="C36" s="2"/>
+    </row>
+    <row r="37" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B37" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C37" s="2"/>
+    </row>
+    <row r="40" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B40" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="C40" s="2">
+        <f>COUNTA(F4:F19)</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="41" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B41" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="C41" s="2">
+        <f>COUNTIF(F4:F19,"Completed")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B42" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="C42" s="2">
+        <f>C40-C41</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="45" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B45" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="C45" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="D45" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="E45" s="9" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="46" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B46" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C46" s="2">
+        <f>COUNTIF(D4:D19,B46)</f>
+        <v>3</v>
+      </c>
+      <c r="D46" s="2">
+        <v>5</v>
+      </c>
+      <c r="E46" s="10">
+        <f>D46/C46</f>
+        <v>1.6666666666666667</v>
+      </c>
+    </row>
+    <row r="47" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B47" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C47" s="2">
+        <f>COUNTIF(D4:D19,B47)</f>
+        <v>2</v>
+      </c>
+      <c r="D47" s="2">
+        <v>3</v>
+      </c>
+      <c r="E47" s="10">
+        <f t="shared" ref="E47:E49" si="0">D47/C47</f>
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="48" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B48" s="2"/>
+      <c r="C48" s="2"/>
+      <c r="D48" s="2"/>
+      <c r="E48" s="10"/>
+    </row>
+    <row r="49" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B49" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C49" s="2">
+        <f>COUNTIF(D4:D19,B49)</f>
+        <v>5</v>
+      </c>
+      <c r="D49" s="2">
+        <v>0</v>
+      </c>
+      <c r="E49" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F4:F22">
+      <formula1>"New, In process, Waiting for Approval, Completed"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D4:D22">
+      <formula1>"MinhKH, KhangTN, ThiTD, TungTD"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
update sprint 3 backlog status
</commit_message>
<xml_diff>
--- a/QA Backlog.xlsx
+++ b/QA Backlog.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="153">
   <si>
     <t>No</t>
   </si>
@@ -434,9 +434,6 @@
     <t>Implement search function</t>
   </si>
   <si>
-    <t>Implement upload and manage material</t>
-  </si>
-  <si>
     <t>Implement follow/unfollow teacher function</t>
   </si>
   <si>
@@ -470,10 +467,16 @@
     <t>solr</t>
   </si>
   <si>
-    <t>Design Manage material UI</t>
-  </si>
-  <si>
-    <t>Design Manage Material UI</t>
+    <t>Design Manage material</t>
+  </si>
+  <si>
+    <t>design add to folder popup and create folder popup</t>
+  </si>
+  <si>
+    <t>Implement upload, add to folder and manage material</t>
+  </si>
+  <si>
+    <t>-na-</t>
   </si>
 </sst>
 </file>
@@ -594,7 +597,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -622,6 +625,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -726,7 +730,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -756,7 +759,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -832,11 +834,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="54149120"/>
-        <c:axId val="76039872"/>
+        <c:axId val="47494656"/>
+        <c:axId val="113838336"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="54149120"/>
+        <c:axId val="47494656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -846,7 +848,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="76039872"/>
+        <c:crossAx val="113838336"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -854,7 +856,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="76039872"/>
+        <c:axId val="113838336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -865,14 +867,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="54149120"/>
+        <c:crossAx val="47494656"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1074,11 +1075,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="54151168"/>
-        <c:axId val="76042752"/>
+        <c:axId val="46235648"/>
+        <c:axId val="113841216"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="54151168"/>
+        <c:axId val="46235648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1088,7 +1089,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="76042752"/>
+        <c:crossAx val="113841216"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1096,7 +1097,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="76042752"/>
+        <c:axId val="113841216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1107,7 +1108,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="54151168"/>
+        <c:crossAx val="46235648"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1194,10 +1195,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>8</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1297,7 +1298,7 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.83333333333333337</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>1</c:v>
@@ -1318,11 +1319,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="59510784"/>
-        <c:axId val="76045632"/>
+        <c:axId val="46237184"/>
+        <c:axId val="45989888"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="59510784"/>
+        <c:axId val="46237184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1332,7 +1333,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="76045632"/>
+        <c:crossAx val="45989888"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1340,7 +1341,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="76045632"/>
+        <c:axId val="45989888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1351,7 +1352,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="59510784"/>
+        <c:crossAx val="46237184"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1562,11 +1563,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="98111488"/>
-        <c:axId val="97951744"/>
+        <c:axId val="96279552"/>
+        <c:axId val="45992768"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="98111488"/>
+        <c:axId val="96279552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1576,7 +1577,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="97951744"/>
+        <c:crossAx val="45992768"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1584,7 +1585,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="97951744"/>
+        <c:axId val="45992768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1595,7 +1596,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="98111488"/>
+        <c:crossAx val="96279552"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2179,7 +2180,7 @@
   <dimension ref="A1:C24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="A13" sqref="A13:XFD13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3206,7 +3207,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M49"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
@@ -3936,8 +3937,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="D49" sqref="D49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4148,9 +4149,15 @@
         <v>86</v>
       </c>
       <c r="G8" s="14"/>
-      <c r="H8" s="14"/>
-      <c r="I8" s="14"/>
-      <c r="J8" s="14"/>
+      <c r="H8" s="14">
+        <v>8</v>
+      </c>
+      <c r="I8" s="14">
+        <v>4</v>
+      </c>
+      <c r="J8" s="14">
+        <v>0</v>
+      </c>
       <c r="K8" s="14"/>
       <c r="L8" s="14"/>
       <c r="M8" s="14"/>
@@ -4284,10 +4291,18 @@
       </c>
       <c r="G13" s="14"/>
       <c r="H13" s="14"/>
-      <c r="I13" s="14"/>
-      <c r="J13" s="14"/>
-      <c r="K13" s="14"/>
-      <c r="L13" s="14"/>
+      <c r="I13" s="14">
+        <v>4</v>
+      </c>
+      <c r="J13" s="14">
+        <v>4</v>
+      </c>
+      <c r="K13" s="14">
+        <v>4</v>
+      </c>
+      <c r="L13" s="14">
+        <v>0</v>
+      </c>
       <c r="M13" s="14"/>
     </row>
     <row r="14" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.2">
@@ -4295,7 +4310,7 @@
         <v>11</v>
       </c>
       <c r="B14" s="14" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C14" s="14"/>
       <c r="D14" s="14" t="s">
@@ -4309,28 +4324,38 @@
       </c>
       <c r="G14" s="14"/>
       <c r="H14" s="14"/>
-      <c r="I14" s="14"/>
-      <c r="J14" s="14"/>
-      <c r="K14" s="14"/>
-      <c r="L14" s="14"/>
-      <c r="M14" s="14"/>
+      <c r="I14" s="14">
+        <v>2</v>
+      </c>
+      <c r="J14" s="14">
+        <v>2</v>
+      </c>
+      <c r="K14" s="14">
+        <v>2</v>
+      </c>
+      <c r="L14" s="14">
+        <v>6</v>
+      </c>
+      <c r="M14" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="15" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="20">
         <v>12</v>
       </c>
       <c r="B15" s="14" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C15" s="14"/>
       <c r="D15" s="14" t="s">
         <v>52</v>
       </c>
       <c r="E15" s="14">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="F15" s="14" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="G15" s="14"/>
       <c r="H15" s="14"/>
@@ -4480,7 +4505,7 @@
       </c>
       <c r="C27" s="2">
         <f>SUMIF(D4:D22,B27,E4:E22)</f>
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.2">
@@ -4555,7 +4580,7 @@
       </c>
       <c r="C41" s="2">
         <f>COUNTIF(F4:F19,"Completed")</f>
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="42" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -4564,7 +4589,7 @@
       </c>
       <c r="C42" s="2">
         <f>C40-C41</f>
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="45" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -4590,11 +4615,11 @@
         <v>6</v>
       </c>
       <c r="D46" s="2">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E46" s="10">
         <f>D46/C46</f>
-        <v>0.83333333333333337</v>
+        <v>1</v>
       </c>
     </row>
     <row r="47" spans="2:5" x14ac:dyDescent="0.2">
@@ -4655,7 +4680,7 @@
   <dimension ref="A1:M49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4736,7 +4761,7 @@
         <v>137</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>52</v>
@@ -4760,9 +4785,11 @@
         <v>2</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="C5" s="2"/>
+        <v>151</v>
+      </c>
+      <c r="C5" s="23" t="s">
+        <v>152</v>
+      </c>
       <c r="D5" s="2" t="s">
         <v>73</v>
       </c>
@@ -4785,9 +4812,11 @@
         <v>3</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>139</v>
-      </c>
-      <c r="C6" s="2"/>
+        <v>138</v>
+      </c>
+      <c r="C6" s="23" t="s">
+        <v>152</v>
+      </c>
       <c r="D6" s="2" t="s">
         <v>75</v>
       </c>
@@ -4810,9 +4839,11 @@
         <v>4</v>
       </c>
       <c r="B7" s="15" t="s">
-        <v>140</v>
-      </c>
-      <c r="C7" s="14"/>
+        <v>139</v>
+      </c>
+      <c r="C7" s="23" t="s">
+        <v>152</v>
+      </c>
       <c r="D7" s="14" t="s">
         <v>75</v>
       </c>
@@ -4835,9 +4866,11 @@
         <v>5</v>
       </c>
       <c r="B8" s="14" t="s">
-        <v>141</v>
-      </c>
-      <c r="C8" s="14"/>
+        <v>140</v>
+      </c>
+      <c r="C8" s="23" t="s">
+        <v>152</v>
+      </c>
       <c r="D8" s="2" t="s">
         <v>75</v>
       </c>
@@ -4860,9 +4893,11 @@
         <v>6</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="C9" s="2"/>
+        <v>141</v>
+      </c>
+      <c r="C9" s="23" t="s">
+        <v>152</v>
+      </c>
       <c r="D9" s="2" t="s">
         <v>75</v>
       </c>
@@ -4885,10 +4920,10 @@
         <v>7</v>
       </c>
       <c r="B10" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>143</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>144</v>
       </c>
       <c r="D10" s="14" t="s">
         <v>73</v>
@@ -4912,10 +4947,10 @@
         <v>8</v>
       </c>
       <c r="B11" s="14" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D11" s="14" t="s">
         <v>75</v>
@@ -4939,9 +4974,11 @@
         <v>9</v>
       </c>
       <c r="B12" s="14" t="s">
-        <v>147</v>
-      </c>
-      <c r="C12" s="13"/>
+        <v>146</v>
+      </c>
+      <c r="C12" s="23" t="s">
+        <v>152</v>
+      </c>
       <c r="D12" s="14" t="s">
         <v>52</v>
       </c>
@@ -4964,9 +5001,11 @@
         <v>10</v>
       </c>
       <c r="B13" s="14" t="s">
-        <v>151</v>
-      </c>
-      <c r="C13" s="14"/>
+        <v>150</v>
+      </c>
+      <c r="C13" s="23" t="s">
+        <v>152</v>
+      </c>
       <c r="D13" s="14" t="s">
         <v>52</v>
       </c>
@@ -4974,7 +5013,7 @@
         <v>4</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>85</v>
+        <v>126</v>
       </c>
       <c r="G13" s="14"/>
       <c r="H13" s="14"/>

</xml_diff>

<commit_message>
update TungTD task status
</commit_message>
<xml_diff>
--- a/QA Backlog.xlsx
+++ b/QA Backlog.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TaDucTung\University\Document\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="240" yWindow="60" windowWidth="15120" windowHeight="8010" activeTab="6"/>
   </bookViews>
@@ -15,7 +20,7 @@
     <sheet name="Sprint 5" sheetId="7" r:id="rId6"/>
     <sheet name="Sprint 6" sheetId="8" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="144525" concurrentCalc="0"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
 </workbook>
 </file>
 
@@ -974,11 +979,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="40403968"/>
-        <c:axId val="40016640"/>
+        <c:axId val="228543616"/>
+        <c:axId val="228544176"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="40403968"/>
+        <c:axId val="228543616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -988,7 +993,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="40016640"/>
+        <c:crossAx val="228544176"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -996,7 +1001,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="40016640"/>
+        <c:axId val="228544176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1007,7 +1012,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="40403968"/>
+        <c:crossAx val="228543616"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1147,7 +1152,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1217,11 +1221,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="40972800"/>
-        <c:axId val="40765120"/>
+        <c:axId val="229249024"/>
+        <c:axId val="229249584"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="40972800"/>
+        <c:axId val="229249024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1231,7 +1235,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="40765120"/>
+        <c:crossAx val="229249584"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1239,7 +1243,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="40765120"/>
+        <c:axId val="229249584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1250,14 +1254,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="40972800"/>
+        <c:crossAx val="229249024"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1362,11 +1365,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="50677248"/>
-        <c:axId val="113249664"/>
+        <c:axId val="228308080"/>
+        <c:axId val="228308640"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="50677248"/>
+        <c:axId val="228308080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1376,7 +1379,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="113249664"/>
+        <c:crossAx val="228308640"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1384,7 +1387,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="113249664"/>
+        <c:axId val="228308640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1395,7 +1398,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="50677248"/>
+        <c:crossAx val="228308080"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1601,11 +1604,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="40099840"/>
-        <c:axId val="113252544"/>
+        <c:axId val="228312560"/>
+        <c:axId val="228313120"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="40099840"/>
+        <c:axId val="228312560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1615,7 +1618,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="113252544"/>
+        <c:crossAx val="228313120"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1623,7 +1626,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="113252544"/>
+        <c:axId val="228313120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1634,7 +1637,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="40099840"/>
+        <c:crossAx val="228312560"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1840,11 +1843,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="40101376"/>
-        <c:axId val="40010880"/>
+        <c:axId val="228630336"/>
+        <c:axId val="228630896"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="40101376"/>
+        <c:axId val="228630336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1854,7 +1857,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="40010880"/>
+        <c:crossAx val="228630896"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1862,7 +1865,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="40010880"/>
+        <c:axId val="228630896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1873,7 +1876,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="40101376"/>
+        <c:crossAx val="228630336"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1933,9 +1936,7 @@
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="1"/>
             <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
-              </c:ext>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
             </c:extLst>
           </c:dLbls>
           <c:cat>
@@ -2081,11 +2082,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="95693824"/>
-        <c:axId val="40013760"/>
+        <c:axId val="228634816"/>
+        <c:axId val="228635376"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="95693824"/>
+        <c:axId val="228634816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2095,7 +2096,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="40013760"/>
+        <c:crossAx val="228635376"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2103,7 +2104,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="40013760"/>
+        <c:axId val="228635376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2114,7 +2115,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="95693824"/>
+        <c:crossAx val="228634816"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2174,9 +2175,7 @@
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="1"/>
             <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
-              </c:ext>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
             </c:extLst>
           </c:dLbls>
           <c:cat>
@@ -2691,7 +2690,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2726,7 +2725,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -6996,15 +6995,15 @@
   <sheetPr codeName="Sheet7"/>
   <dimension ref="A1:M49"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="1"/>
     <col min="2" max="2" width="56.7109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="20.5703125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="64.85546875" style="1" customWidth="1"/>
     <col min="4" max="4" width="14.42578125" style="1" customWidth="1"/>
     <col min="5" max="5" width="18" style="1" customWidth="1"/>
     <col min="6" max="6" width="21.7109375" style="1" customWidth="1"/>
@@ -7242,7 +7241,7 @@
         <v>6</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>165</v>
+        <v>125</v>
       </c>
       <c r="G10" s="14"/>
       <c r="H10" s="14"/>
@@ -7267,7 +7266,7 @@
         <v>6</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>165</v>
+        <v>125</v>
       </c>
       <c r="G11" s="14"/>
       <c r="H11" s="14"/>
@@ -7294,7 +7293,7 @@
         <v>10</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>165</v>
+        <v>125</v>
       </c>
       <c r="G12" s="14"/>
       <c r="H12" s="14"/>
@@ -7321,7 +7320,7 @@
         <v>6</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>165</v>
+        <v>82</v>
       </c>
       <c r="G13" s="14"/>
       <c r="H13" s="14"/>

</xml_diff>

<commit_message>
update task status tungtd
</commit_message>
<xml_diff>
--- a/QA Backlog.xlsx
+++ b/QA Backlog.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TaDucTung\University\Document\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="240" yWindow="60" windowWidth="15120" windowHeight="8010" activeTab="6"/>
   </bookViews>
@@ -15,7 +20,7 @@
     <sheet name="Sprint 5" sheetId="7" r:id="rId6"/>
     <sheet name="Sprint 6" sheetId="8" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="144525" concurrentCalc="0"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
 </workbook>
 </file>
 
@@ -974,11 +979,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="116223488"/>
-        <c:axId val="50387712"/>
+        <c:axId val="292352144"/>
+        <c:axId val="292362224"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="116223488"/>
+        <c:axId val="292352144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -988,7 +993,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="50387712"/>
+        <c:crossAx val="292362224"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -996,7 +1001,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="50387712"/>
+        <c:axId val="292362224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1007,7 +1012,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="116223488"/>
+        <c:crossAx val="292352144"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1147,6 +1152,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1216,11 +1222,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="116628992"/>
-        <c:axId val="117196480"/>
+        <c:axId val="292826704"/>
+        <c:axId val="292827264"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="116628992"/>
+        <c:axId val="292826704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1230,7 +1236,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="117196480"/>
+        <c:crossAx val="292827264"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1238,7 +1244,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="117196480"/>
+        <c:axId val="292827264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1249,13 +1255,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="116628992"/>
+        <c:crossAx val="292826704"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1360,11 +1367,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="50184704"/>
-        <c:axId val="66891136"/>
+        <c:axId val="226616848"/>
+        <c:axId val="226617408"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="50184704"/>
+        <c:axId val="226616848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1374,7 +1381,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="66891136"/>
+        <c:crossAx val="226617408"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1382,7 +1389,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="66891136"/>
+        <c:axId val="226617408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1393,7 +1400,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="50184704"/>
+        <c:crossAx val="226616848"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1599,11 +1606,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="50186240"/>
-        <c:axId val="66894016"/>
+        <c:axId val="228238800"/>
+        <c:axId val="228239360"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="50186240"/>
+        <c:axId val="228238800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1613,7 +1620,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="66894016"/>
+        <c:crossAx val="228239360"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1621,7 +1628,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="66894016"/>
+        <c:axId val="228239360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1632,7 +1639,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="50186240"/>
+        <c:crossAx val="228238800"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1838,11 +1845,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="116219904"/>
-        <c:axId val="50381952"/>
+        <c:axId val="227946080"/>
+        <c:axId val="227946640"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="116219904"/>
+        <c:axId val="227946080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1852,7 +1859,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="50381952"/>
+        <c:crossAx val="227946640"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1860,7 +1867,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="50381952"/>
+        <c:axId val="227946640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1871,7 +1878,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="116219904"/>
+        <c:crossAx val="227946080"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2077,11 +2084,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="116221440"/>
-        <c:axId val="50384832"/>
+        <c:axId val="228051904"/>
+        <c:axId val="228052464"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="116221440"/>
+        <c:axId val="228051904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2091,7 +2098,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="50384832"/>
+        <c:crossAx val="228052464"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2099,7 +2106,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="50384832"/>
+        <c:axId val="228052464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2110,7 +2117,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="116221440"/>
+        <c:crossAx val="228051904"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2685,7 +2692,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2720,7 +2727,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -6990,8 +6997,8 @@
   <sheetPr codeName="Sheet7"/>
   <dimension ref="A1:M49"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M27" sqref="M27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -7211,13 +7218,27 @@
       <c r="F9" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="G9" s="14"/>
-      <c r="H9" s="14"/>
-      <c r="I9" s="14"/>
-      <c r="J9" s="14"/>
-      <c r="K9" s="14"/>
-      <c r="L9" s="14"/>
-      <c r="M9" s="14"/>
+      <c r="G9" s="14">
+        <v>2</v>
+      </c>
+      <c r="H9" s="14">
+        <v>2</v>
+      </c>
+      <c r="I9" s="14">
+        <v>0</v>
+      </c>
+      <c r="J9" s="14">
+        <v>0</v>
+      </c>
+      <c r="K9" s="14">
+        <v>0</v>
+      </c>
+      <c r="L9" s="14">
+        <v>0</v>
+      </c>
+      <c r="M9" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="10" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="14">
@@ -7238,13 +7259,27 @@
       <c r="F10" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="G10" s="14"/>
-      <c r="H10" s="14"/>
-      <c r="I10" s="14"/>
-      <c r="J10" s="14"/>
-      <c r="K10" s="14"/>
-      <c r="L10" s="14"/>
-      <c r="M10" s="14"/>
+      <c r="G10" s="14">
+        <v>3</v>
+      </c>
+      <c r="H10" s="14">
+        <v>3</v>
+      </c>
+      <c r="I10" s="14">
+        <v>2</v>
+      </c>
+      <c r="J10" s="14">
+        <v>0</v>
+      </c>
+      <c r="K10" s="14">
+        <v>0</v>
+      </c>
+      <c r="L10" s="14">
+        <v>0</v>
+      </c>
+      <c r="M10" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="11" spans="1:13" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="11">
@@ -7266,10 +7301,18 @@
       <c r="G11" s="11"/>
       <c r="H11" s="11"/>
       <c r="I11" s="11"/>
-      <c r="J11" s="11"/>
-      <c r="K11" s="11"/>
-      <c r="L11" s="11"/>
-      <c r="M11" s="11"/>
+      <c r="J11" s="11">
+        <v>3</v>
+      </c>
+      <c r="K11" s="11">
+        <v>3</v>
+      </c>
+      <c r="L11" s="11">
+        <v>3</v>
+      </c>
+      <c r="M11" s="11">
+        <v>2</v>
+      </c>
     </row>
     <row r="12" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="14">
@@ -7291,12 +7334,24 @@
         <v>125</v>
       </c>
       <c r="G12" s="14"/>
-      <c r="H12" s="14"/>
-      <c r="I12" s="14"/>
-      <c r="J12" s="14"/>
-      <c r="K12" s="14"/>
-      <c r="L12" s="14"/>
-      <c r="M12" s="14"/>
+      <c r="H12" s="14">
+        <v>1</v>
+      </c>
+      <c r="I12" s="14">
+        <v>3</v>
+      </c>
+      <c r="J12" s="14">
+        <v>3</v>
+      </c>
+      <c r="K12" s="14">
+        <v>3</v>
+      </c>
+      <c r="L12" s="14">
+        <v>0</v>
+      </c>
+      <c r="M12" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="13" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="14">
@@ -7315,15 +7370,19 @@
         <v>6</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>82</v>
+        <v>125</v>
       </c>
       <c r="G13" s="14"/>
       <c r="H13" s="14"/>
       <c r="I13" s="14"/>
       <c r="J13" s="14"/>
       <c r="K13" s="14"/>
-      <c r="L13" s="14"/>
-      <c r="M13" s="14"/>
+      <c r="L13" s="14">
+        <v>3</v>
+      </c>
+      <c r="M13" s="14">
+        <v>3</v>
+      </c>
     </row>
     <row r="14" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="14">

</xml_diff>